<commit_message>
Swap household contact information for parents
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0A3D9BC-DD64-497A-9BA3-73C8AB5D057E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A109CA-6EDE-4924-BD5A-E76BD23D13A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="1108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="1117">
   <si>
     <t>vars</t>
   </si>
@@ -3366,6 +3366,33 @@
   </si>
   <si>
     <t>part_ethnicity2</t>
+  </si>
+  <si>
+    <t>cnt_prec_none</t>
+  </si>
+  <si>
+    <t>cnt_prec_dk</t>
+  </si>
+  <si>
+    <t>cnt_prec_2m_plus</t>
+  </si>
+  <si>
+    <t>cnt_prec_1m_plus</t>
+  </si>
+  <si>
+    <t>cnt_prec_within_1m</t>
+  </si>
+  <si>
+    <t>cnt_prec_mask</t>
+  </si>
+  <si>
+    <t>cnt_prec_wash_before</t>
+  </si>
+  <si>
+    <t>cnt_prec_wash_after</t>
+  </si>
+  <si>
+    <t>cnt_prec_prefer_not_to_say</t>
   </si>
 </sst>
 </file>
@@ -3726,8 +3753,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:K650"/>
   <sheetViews>
-    <sheetView topLeftCell="A558" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B649"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -20620,11 +20647,11 @@
         <v>1</v>
       </c>
       <c r="J497">
-        <f t="shared" si="14"/>
+        <f>SUM(C497:F497)</f>
         <v>0</v>
       </c>
       <c r="K497">
-        <f t="shared" si="15"/>
+        <f>SUM(G497:H497)</f>
         <v>2</v>
       </c>
     </row>
@@ -25840,6 +25867,9 @@
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="J19:J25 J26 J27:J649 K19:K25 K1:K18 K26:K649" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
@@ -25847,8 +25877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1C5985-D720-4533-B6F5-A2816F80F2F5}">
   <dimension ref="A1:B418"/>
   <sheetViews>
-    <sheetView topLeftCell="A293" workbookViewId="0">
-      <selection activeCell="B321" sqref="B321"/>
+    <sheetView topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29214,8 +29244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6804872F-908E-4576-8C9F-D057085582A0}">
   <dimension ref="A1:B256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="B155" sqref="B155"/>
+    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+      <selection activeCell="B197" sqref="B197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -30633,7 +30663,7 @@
         <v>485</v>
       </c>
       <c r="B177" t="s">
-        <v>989</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.45">
@@ -30641,7 +30671,7 @@
         <v>486</v>
       </c>
       <c r="B178" t="s">
-        <v>1106</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.45">
@@ -30649,7 +30679,7 @@
         <v>487</v>
       </c>
       <c r="B179" t="s">
-        <v>990</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.45">
@@ -30657,7 +30687,7 @@
         <v>488</v>
       </c>
       <c r="B180" t="s">
-        <v>991</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.45">
@@ -30665,7 +30695,7 @@
         <v>489</v>
       </c>
       <c r="B181" t="s">
-        <v>992</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.45">
@@ -30673,7 +30703,7 @@
         <v>490</v>
       </c>
       <c r="B182" t="s">
-        <v>993</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.45">
@@ -30681,7 +30711,7 @@
         <v>491</v>
       </c>
       <c r="B183" t="s">
-        <v>994</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.45">
@@ -30689,7 +30719,7 @@
         <v>492</v>
       </c>
       <c r="B184" t="s">
-        <v>995</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.45">
@@ -30697,7 +30727,7 @@
         <v>493</v>
       </c>
       <c r="B185" t="s">
-        <v>996</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.45">
@@ -31279,7 +31309,7 @@
   <dimension ref="A1:B223"/>
   <sheetViews>
     <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127"/>
+      <selection activeCell="B127" sqref="B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Update contact clean with dates
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A109CA-6EDE-4924-BD5A-E76BD23D13A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8289867-E8A4-4376-B189-9DB799804011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
@@ -16,7 +16,8 @@
     <sheet name="All_vars" sheetId="1" r:id="rId1"/>
     <sheet name="survey_1" sheetId="2" r:id="rId2"/>
     <sheet name="survey_2" sheetId="3" r:id="rId3"/>
-    <sheet name="oldsheet_v2" sheetId="4" r:id="rId4"/>
+    <sheet name="locations" sheetId="5" r:id="rId4"/>
+    <sheet name="oldsheet_v2" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">All_vars!$A$1:$K$650</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="1117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2628" uniqueCount="1166">
   <si>
     <t>vars</t>
   </si>
@@ -3393,6 +3394,153 @@
   </si>
   <si>
     <t>cnt_prec_prefer_not_to_say</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>Northern Irel</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>Région Flamande / Vlaams Gewest</t>
+  </si>
+  <si>
+    <t>Région Wallonne / Waals Gewest</t>
+  </si>
+  <si>
+    <t>Région de Bruxelles-Capitale / Brussels Hoofdstede</t>
+  </si>
+  <si>
+    <t>Région de Bruxelles-Capitale / Brussels Hoofdsted</t>
+  </si>
+  <si>
+    <t>nl</t>
+  </si>
+  <si>
+    <t>Oost-Nederland</t>
+  </si>
+  <si>
+    <t>Noord-Nederland</t>
+  </si>
+  <si>
+    <t>Zuid-Nederland</t>
+  </si>
+  <si>
+    <t>West-Nederland</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Akershus</t>
+  </si>
+  <si>
+    <t>Oslo</t>
+  </si>
+  <si>
+    <t>Vestfold</t>
+  </si>
+  <si>
+    <t>Rogaland</t>
+  </si>
+  <si>
+    <t>Hordaland</t>
+  </si>
+  <si>
+    <t>Vest-Agder</t>
+  </si>
+  <si>
+    <t>Nordland</t>
+  </si>
+  <si>
+    <t>Møre og Romsdal</t>
+  </si>
+  <si>
+    <t>Trøndelag</t>
+  </si>
+  <si>
+    <t>Telemark</t>
+  </si>
+  <si>
+    <t>Østfold</t>
+  </si>
+  <si>
+    <t>Buskerud</t>
+  </si>
+  <si>
+    <t>Troms</t>
+  </si>
+  <si>
+    <t>Sogn og Fjordane</t>
+  </si>
+  <si>
+    <t>Finnmark</t>
+  </si>
+  <si>
+    <t>Hedmark</t>
+  </si>
+  <si>
+    <t>Oppland</t>
+  </si>
+  <si>
+    <t>Aust-Agder</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t>South East</t>
+  </si>
+  <si>
+    <t>North West</t>
+  </si>
+  <si>
+    <t>West Midlands</t>
+  </si>
+  <si>
+    <t>East Midlands</t>
+  </si>
+  <si>
+    <t>South West</t>
+  </si>
+  <si>
+    <t>Greater London</t>
+  </si>
+  <si>
+    <t>Wales</t>
+  </si>
+  <si>
+    <t>North East</t>
+  </si>
+  <si>
+    <t>Yorkshire and The Humber</t>
+  </si>
+  <si>
+    <t>Scotland</t>
+  </si>
+  <si>
+    <t>East of England</t>
+  </si>
+  <si>
+    <t>Northern Ireland</t>
+  </si>
+  <si>
+    <t>Yorkshire and Humberside</t>
+  </si>
+  <si>
+    <t>East Anglia</t>
+  </si>
+  <si>
+    <t>Greater Londo</t>
+  </si>
+  <si>
+    <t>Yorkshire and</t>
+  </si>
+  <si>
+    <t>East of Engla</t>
   </si>
 </sst>
 </file>
@@ -25877,8 +26025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1C5985-D720-4533-B6F5-A2816F80F2F5}">
   <dimension ref="A1:B418"/>
   <sheetViews>
-    <sheetView topLeftCell="A271" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26004,7 +26152,7 @@
         <v>309</v>
       </c>
       <c r="B15" t="s">
-        <v>569</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -26012,7 +26160,7 @@
         <v>310</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
@@ -26020,7 +26168,7 @@
         <v>311</v>
       </c>
       <c r="B17" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
@@ -29244,7 +29392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6804872F-908E-4576-8C9F-D057085582A0}">
   <dimension ref="A1:B256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
       <selection activeCell="B197" sqref="B197"/>
     </sheetView>
   </sheetViews>
@@ -29290,7 +29438,7 @@
         <v>309</v>
       </c>
       <c r="B5" t="s">
-        <v>569</v>
+        <v>309</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
@@ -29298,7 +29446,7 @@
         <v>310</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -29306,7 +29454,7 @@
         <v>311</v>
       </c>
       <c r="B7" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -30751,7 +30899,7 @@
         <v>999</v>
       </c>
       <c r="B188" t="s">
-        <v>904</v>
+        <v>910</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.45">
@@ -30783,7 +30931,7 @@
         <v>1003</v>
       </c>
       <c r="B192" t="s">
-        <v>906</v>
+        <v>912</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.45">
@@ -30815,7 +30963,7 @@
         <v>1007</v>
       </c>
       <c r="B196" t="s">
-        <v>908</v>
+        <v>914</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.45">
@@ -31305,6 +31453,659 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6379954C-B519-4E67-8DE4-32A1851A1CD0}">
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="41.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C1" t="s">
+        <v>556</v>
+      </c>
+      <c r="D1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B3" t="s">
+        <v>576</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1120</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B5" t="s">
+        <v>576</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B6" t="s">
+        <v>576</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1126</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B7" t="s">
+        <v>576</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>576</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1128</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B9" t="s">
+        <v>576</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B10" t="s">
+        <v>576</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1130</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B11" t="s">
+        <v>576</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1147</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B12" t="s">
+        <v>576</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1141</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B13" t="s">
+        <v>576</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1144</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B14" t="s">
+        <v>576</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B15" t="s">
+        <v>576</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1134</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B16" t="s">
+        <v>576</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1137</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B17" t="s">
+        <v>576</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B18" t="s">
+        <v>576</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B19" t="s">
+        <v>576</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B20" t="s">
+        <v>576</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B21" t="s">
+        <v>576</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B22" t="s">
+        <v>576</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B23" t="s">
+        <v>576</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1139</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B24" t="s">
+        <v>576</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B25" t="s">
+        <v>576</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B26" t="s">
+        <v>576</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1135</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B27" t="s">
+        <v>576</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B28" t="s">
+        <v>576</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B29" t="s">
+        <v>576</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B30" t="s">
+        <v>576</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1165</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B31" t="s">
+        <v>576</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1159</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B32" t="s">
+        <v>576</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1163</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B33" t="s">
+        <v>576</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B34" t="s">
+        <v>576</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1156</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B35" t="s">
+        <v>576</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B36" t="s">
+        <v>576</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1118</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B37" t="s">
+        <v>576</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1160</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B38" t="s">
+        <v>576</v>
+      </c>
+      <c r="C38" t="s">
+        <v>1158</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B39" t="s">
+        <v>576</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1149</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B40" t="s">
+        <v>576</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1153</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B41" t="s">
+        <v>576</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1155</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B42" t="s">
+        <v>576</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B43" t="s">
+        <v>576</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B44" t="s">
+        <v>576</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1161</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B45" t="s">
+        <v>576</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1157</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C45">
+    <sortCondition ref="A2:A45"/>
+    <sortCondition ref="C2:C45"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1846DEF0-F0AD-422F-BC6D-F9094EDD7D3F}">
   <dimension ref="A1:B223"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add sheet for removing variables
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49597AE9-1ADA-4C16-B006-3BAC5D438E58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70927852-BEAC-4C5F-B1A1-3D1185C56722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="3" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="All_vars" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="survey_2" sheetId="3" r:id="rId3"/>
     <sheet name="locations" sheetId="5" r:id="rId4"/>
     <sheet name="oldsheet_v2" sheetId="4" r:id="rId5"/>
+    <sheet name="remove_vars" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">All_vars!$A$1:$K$650</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="1188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2939" uniqueCount="1389">
   <si>
     <t>vars</t>
   </si>
@@ -3607,6 +3608,609 @@
   </si>
   <si>
     <t>Northern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cultureinfo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">main_intro_screen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">privacypolicy_insert </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_5_name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_pop_dens_1_code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_pop_dens_1_label </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_pop_dens_2_code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_pop_dens_2_label </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_rural_urban_code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_rural_urban_label </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_1_code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_town_label </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_town_code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_town_pop_code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_1_name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_2_code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_2_name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_tv_station </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_3_code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_3_name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_4_code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_4_name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_5_code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sniffer_device_type_final </t>
+  </si>
+  <si>
+    <t xml:space="preserve">sniffer_device_type_initial </t>
+  </si>
+  <si>
+    <t xml:space="preserve">higher_earner_occupation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uksg_version </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q48a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_scale_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q49_l0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">quotagerange </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ukregion1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ukstdregion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">area_town_pop_label </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qsample </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q51 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q20b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_10 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_11 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_12 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_13 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_15 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_16 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_17 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q23_quota_9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q61a_insert </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q61b_codes_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q61b_codes_2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q61b_insert </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q20_new </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q20_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_scale_1_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q20 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">usegendernonbinary </t>
+  </si>
+  <si>
+    <t xml:space="preserve">insq61a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">insq61b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q53a_choosen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q59_7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q61b_codes_98 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q61b_codes_99 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk02eth_18 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">part_ukitv </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ukmktsize </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ukmktsize2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ukmunicipality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk_region1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk_region2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk_region3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk_region3_label </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ukruralurban </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk_stdmktsize </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk_stdregion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk_towncode </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk_townname </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q20_import </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_1_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_2_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_3_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_4_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_5_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_6_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_7_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_8_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_10_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_12_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_13_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_14_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_9_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_15_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_22_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_23_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_24_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_25_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q63validate </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qconfirm1a </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qconfirm1b </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w1_namesexage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w2_namesexage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w3_namesexage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nameagesex_scale_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_32_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_33_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_34_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_35_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w4_namesexage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_42_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_43_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_44_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_45_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w5_namesexage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_52_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_53_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_54_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q21_55_original </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w6_namesexage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">higher_earner_education </t>
+  </si>
+  <si>
+    <t xml:space="preserve">higher_earner_occupation_prev </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q51_help_3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q50_help_3 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q41 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q40 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q39 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q26_filter_8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q_panel </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q_wave </t>
+  </si>
+  <si>
+    <t xml:space="preserve">bestdregion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q49_l1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ical_standardoccupation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">nostdregion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">q36_insert_4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qedu_no </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qforigin_codes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qforigin_rec </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmorigin_codes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmorigin_rec </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qn086 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qno81 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qrorigin_codes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qrorigin_rec </t>
+  </si>
+  <si>
+    <t>check_to_remove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_refused_to_answer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_text </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsizeversion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_15_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_16_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_32_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_33_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_44_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_45_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_46_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_47_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_48_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_49_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_50_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_51_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_52_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_53_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_54_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_55_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_57_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_58_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_59_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_60_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_61_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_62_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_63_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_64_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_65_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_66_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_67_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_68_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_69_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_70_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_71_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_72_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_73_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_74_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_75_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_76_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_77_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_78_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_79_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_80_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_81_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_82_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_19_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_85_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_86_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_34_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_35_1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">qmktsize_36_1 </t>
+  </si>
+  <si>
+    <t>remove</t>
   </si>
 </sst>
 </file>
@@ -26083,8 +26687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1C5985-D720-4533-B6F5-A2816F80F2F5}">
   <dimension ref="A1:B418"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A385" sqref="A385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31514,7 +32118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6379954C-B519-4E67-8DE4-32A1851A1CD0}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D56" sqref="D56:D73"/>
     </sheetView>
   </sheetViews>
@@ -34351,4 +34955,856 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB4B1FA-6628-4BA2-9F29-B27CBB154F46}">
+  <dimension ref="A1:B111"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="36.1328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>1212</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1277</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1278</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B70" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B71" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B72" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B73" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B77" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B78" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B79" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B91" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
+        <v>229</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B93" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B94" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B95" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B96" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B97" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B98" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B99" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B100" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B101" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B102" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B103" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B104" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B105" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B106" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B107" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B108" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B109" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B110" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B111" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A484">
+    <sortCondition ref="A2:A484"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add new var_names remove duplicates
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70927852-BEAC-4C5F-B1A1-3D1185C56722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA5A986-D2FD-4E9D-B1BA-3BF86F207699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
-    <sheet name="All_vars" sheetId="1" r:id="rId1"/>
-    <sheet name="survey_1" sheetId="2" r:id="rId2"/>
-    <sheet name="survey_2" sheetId="3" r:id="rId3"/>
-    <sheet name="locations" sheetId="5" r:id="rId4"/>
-    <sheet name="oldsheet_v2" sheetId="4" r:id="rId5"/>
-    <sheet name="remove_vars" sheetId="6" r:id="rId6"/>
+    <sheet name="Summary" sheetId="7" r:id="rId1"/>
+    <sheet name="All_vars" sheetId="1" r:id="rId2"/>
+    <sheet name="survey_1" sheetId="2" r:id="rId3"/>
+    <sheet name="survey_2" sheetId="3" r:id="rId4"/>
+    <sheet name="locations" sheetId="5" r:id="rId5"/>
+    <sheet name="oldsheet_v2" sheetId="4" r:id="rId6"/>
+    <sheet name="remove_vars" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">All_vars!$A$1:$K$650</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">survey_1!$A$1:$G$423</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">survey_2!$A$1:$B$262</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">All_vars!$A$1:$K$650</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">survey_1!$A$1:$G$423</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">survey_2!$A$1:$B$262</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4567,6 +4568,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED087E4C-9F1F-4889-910F-E633D6596E81}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59DB8823-33FC-4C68-8AB1-65768017318F}">
   <dimension ref="A1:K650"/>
   <sheetViews>
@@ -4634,11 +4647,11 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J19" si="0">SUM(C2:F2)</f>
+        <f t="shared" ref="J2" si="0">SUM(C2:F2)</f>
         <v>1</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K19" si="1">SUM(G2:H2)</f>
+        <f t="shared" ref="K2" si="1">SUM(G2:H2)</f>
         <v>0</v>
       </c>
     </row>
@@ -26683,7 +26696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1C5985-D720-4533-B6F5-A2816F80F2F5}">
   <dimension ref="A1:B418"/>
   <sheetViews>
@@ -30050,7 +30063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6804872F-908E-4576-8C9F-D057085582A0}">
   <dimension ref="A1:B256"/>
   <sheetViews>
@@ -32114,11 +32127,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6379954C-B519-4E67-8DE4-32A1851A1CD0}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D56" sqref="D56:D73"/>
     </sheetView>
   </sheetViews>
@@ -33164,7 +33177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1846DEF0-F0AD-422F-BC6D-F9094EDD7D3F}">
   <dimension ref="A1:B223"/>
   <sheetViews>
@@ -34957,11 +34970,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB4B1FA-6628-4BA2-9F29-B27CBB154F46}">
   <dimension ref="A1:B111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+    <sheetView topLeftCell="A60" workbookViewId="0">
       <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Edited var name closes #4
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA5A986-D2FD-4E9D-B1BA-3BF86F207699}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118BEFFD-1DB2-495A-BB56-5155C20F3BAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2939" uniqueCount="1389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2940" uniqueCount="1390">
   <si>
     <t>vars</t>
   </si>
@@ -4212,6 +4212,9 @@
   </si>
   <si>
     <t>remove</t>
+  </si>
+  <si>
+    <t>List variable names and way of cleaning the locations</t>
   </si>
 </sst>
 </file>
@@ -4569,12 +4572,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED087E4C-9F1F-4889-910F-E633D6596E81}">
-  <dimension ref="A1"/>
+  <dimension ref="A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Edited var name closes #3
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{118BEFFD-1DB2-495A-BB56-5155C20F3BAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC423AE8-646E-4E9D-85B2-443C38A13A8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2940" uniqueCount="1390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2941" uniqueCount="1391">
   <si>
     <t>vars</t>
   </si>
@@ -4215,6 +4215,9 @@
   </si>
   <si>
     <t>List variable names and way of cleaning the locations</t>
+  </si>
+  <si>
+    <t>Need to add different ones for different surveys</t>
   </si>
 </sst>
 </file>
@@ -4572,10 +4575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED087E4C-9F1F-4889-910F-E633D6596E81}">
-  <dimension ref="A3"/>
+  <dimension ref="A3:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4583,6 +4586,11 @@
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1389</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>1390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove phys to cnt_phys
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C79F556-9FB1-4B59-BCC6-A643A632ACB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54622D8-2032-4094-A8D8-3A5212996204}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13118" yWindow="195" windowWidth="15195" windowHeight="15450" activeTab="3" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="9225" yWindow="487" windowWidth="15195" windowHeight="15450" activeTab="3" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2941" uniqueCount="1391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2941" uniqueCount="1392">
   <si>
     <t>vars</t>
   </si>
@@ -4218,6 +4218,9 @@
   </si>
   <si>
     <t>cnt_other_place</t>
+  </si>
+  <si>
+    <t>hhm_contact</t>
   </si>
 </sst>
 </file>
@@ -26719,8 +26722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1C5985-D720-4533-B6F5-A2816F80F2F5}">
   <dimension ref="A1:B418"/>
   <sheetViews>
-    <sheetView topLeftCell="A300" workbookViewId="0">
-      <selection activeCell="B325" sqref="B325"/>
+    <sheetView topLeftCell="A330" workbookViewId="0">
+      <selection activeCell="B358" sqref="B358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29230,7 +29233,7 @@
         <v>455</v>
       </c>
       <c r="B313" t="s">
-        <v>838</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.45">
@@ -29286,7 +29289,7 @@
         <v>210</v>
       </c>
       <c r="B320" t="s">
-        <v>844</v>
+        <v>975</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.45">
@@ -30086,8 +30089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6804872F-908E-4576-8C9F-D057085582A0}">
   <dimension ref="A1:B256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="B148" sqref="B148"/>
+    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31265,7 +31268,7 @@
         <v>455</v>
       </c>
       <c r="B147" t="s">
-        <v>838</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Update names of visit vars
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54622D8-2032-4094-A8D8-3A5212996204}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CBE19E-7691-4D8A-8925-08B7C2240BE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9225" yWindow="487" windowWidth="15195" windowHeight="15450" activeTab="3" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2941" uniqueCount="1392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2941" uniqueCount="1401">
   <si>
     <t>vars</t>
   </si>
@@ -4221,6 +4221,33 @@
   </si>
   <si>
     <t>hhm_contact</t>
+  </si>
+  <si>
+    <t>part_visit_another_home_int</t>
+  </si>
+  <si>
+    <t>part_visit_salon_int</t>
+  </si>
+  <si>
+    <t>part_visit_none_int</t>
+  </si>
+  <si>
+    <t>part_visit_public_transport_int</t>
+  </si>
+  <si>
+    <t>part_visit_essential_shop_int</t>
+  </si>
+  <si>
+    <t>part_visit_non_essential_shop_int</t>
+  </si>
+  <si>
+    <t>part_visit_sport_venue_int</t>
+  </si>
+  <si>
+    <t>part_visit_outdoors_int</t>
+  </si>
+  <si>
+    <t>part_visit_healthcare_int</t>
   </si>
 </sst>
 </file>
@@ -30089,8 +30116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6804872F-908E-4576-8C9F-D057085582A0}">
   <dimension ref="A1:B256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="B176" sqref="B176"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -30972,7 +30999,7 @@
         <v>417</v>
       </c>
       <c r="B110" t="s">
-        <v>959</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.45">
@@ -30980,7 +31007,7 @@
         <v>418</v>
       </c>
       <c r="B111" t="s">
-        <v>960</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.45">
@@ -30988,7 +31015,7 @@
         <v>419</v>
       </c>
       <c r="B112" t="s">
-        <v>961</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
@@ -30996,7 +31023,7 @@
         <v>420</v>
       </c>
       <c r="B113" t="s">
-        <v>962</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
@@ -31004,7 +31031,7 @@
         <v>421</v>
       </c>
       <c r="B114" t="s">
-        <v>963</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
@@ -31012,7 +31039,7 @@
         <v>422</v>
       </c>
       <c r="B115" t="s">
-        <v>964</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
@@ -31020,7 +31047,7 @@
         <v>423</v>
       </c>
       <c r="B116" t="s">
-        <v>965</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
@@ -31028,7 +31055,7 @@
         <v>424</v>
       </c>
       <c r="B117" t="s">
-        <v>773</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
@@ -31036,7 +31063,7 @@
         <v>425</v>
       </c>
       <c r="B118" t="s">
-        <v>966</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.45">
@@ -31044,7 +31071,7 @@
         <v>426</v>
       </c>
       <c r="B119" t="s">
-        <v>967</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
@@ -31052,7 +31079,7 @@
         <v>427</v>
       </c>
       <c r="B120" t="s">
-        <v>968</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Update for pub rest contacts and latest data
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{832EA055-D935-45ED-A29A-14CDDB73933E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8530E2A-C1F3-4E97-B0DD-BD0CBF576B20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="6" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2941" uniqueCount="1405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2859" uniqueCount="1323">
   <si>
     <t>vars</t>
   </si>
@@ -3569,84 +3569,18 @@
     <t xml:space="preserve">privacypolicy_insert </t>
   </si>
   <si>
-    <t xml:space="preserve">area_5_name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_pop_dens_1_code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_pop_dens_1_label </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_pop_dens_2_code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_pop_dens_2_label </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_rural_urban_code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_rural_urban_label </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_1_code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_town_label </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_town_code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_town_pop_code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_1_name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_2_code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_2_name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_tv_station </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_3_code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_3_name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_4_code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_4_name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">area_5_code </t>
-  </si>
-  <si>
     <t xml:space="preserve">sniffer_device_type_final </t>
   </si>
   <si>
     <t xml:space="preserve">sniffer_device_type_initial </t>
   </si>
   <si>
-    <t xml:space="preserve">higher_earner_occupation </t>
-  </si>
-  <si>
     <t xml:space="preserve">uksg_version </t>
   </si>
   <si>
     <t xml:space="preserve">q48a </t>
   </si>
   <si>
-    <t xml:space="preserve">q21_scale_1 </t>
-  </si>
-  <si>
     <t xml:space="preserve">q49_l0 </t>
   </si>
   <si>
@@ -3659,69 +3593,12 @@
     <t xml:space="preserve">ukstdregion </t>
   </si>
   <si>
-    <t xml:space="preserve">area_town_pop_label </t>
-  </si>
-  <si>
     <t xml:space="preserve">qsample </t>
   </si>
   <si>
-    <t xml:space="preserve">q51 </t>
-  </si>
-  <si>
     <t xml:space="preserve">q20b </t>
   </si>
   <si>
-    <t xml:space="preserve">q23_quota_1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_10 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_11 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_12 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_13 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_14 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_15 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_16 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_17 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_4 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_5 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_6 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_7 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_8 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q23_quota_9 </t>
-  </si>
-  <si>
     <t xml:space="preserve">q61a_insert </t>
   </si>
   <si>
@@ -3740,9 +3617,6 @@
     <t xml:space="preserve">q20_original </t>
   </si>
   <si>
-    <t xml:space="preserve">q21_scale_1_original </t>
-  </si>
-  <si>
     <t xml:space="preserve">q20 </t>
   </si>
   <si>
@@ -3758,9 +3632,6 @@
     <t xml:space="preserve">q53a_choosen </t>
   </si>
   <si>
-    <t xml:space="preserve">q59_7 </t>
-  </si>
-  <si>
     <t xml:space="preserve">q61b_codes_98 </t>
   </si>
   <si>
@@ -3782,90 +3653,15 @@
     <t xml:space="preserve">ukmunicipality </t>
   </si>
   <si>
-    <t xml:space="preserve">uk_region1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">uk_region2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">uk_region3 </t>
-  </si>
-  <si>
     <t xml:space="preserve">uk_region3_label </t>
   </si>
   <si>
     <t xml:space="preserve">ukruralurban </t>
   </si>
   <si>
-    <t xml:space="preserve">uk_stdmktsize </t>
-  </si>
-  <si>
-    <t xml:space="preserve">uk_stdregion </t>
-  </si>
-  <si>
-    <t xml:space="preserve">uk_towncode </t>
-  </si>
-  <si>
-    <t xml:space="preserve">uk_townname </t>
-  </si>
-  <si>
     <t xml:space="preserve">q20_import </t>
   </si>
   <si>
-    <t xml:space="preserve">q21_1_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_2_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_3_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_4_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_5_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_6_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_7_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_8_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_10_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_12_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_13_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_14_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_9_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_15_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_22_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_23_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_24_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_25_original </t>
-  </si>
-  <si>
     <t xml:space="preserve">q63validate </t>
   </si>
   <si>
@@ -3887,63 +3683,15 @@
     <t xml:space="preserve">nameagesex_scale_1 </t>
   </si>
   <si>
-    <t xml:space="preserve">q21_32_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_33_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_34_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_35_original </t>
-  </si>
-  <si>
     <t xml:space="preserve">w4_namesexage </t>
   </si>
   <si>
-    <t xml:space="preserve">q21_42_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_43_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_44_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_45_original </t>
-  </si>
-  <si>
     <t xml:space="preserve">w5_namesexage </t>
   </si>
   <si>
-    <t xml:space="preserve">q21_52_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_53_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_54_original </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q21_55_original </t>
-  </si>
-  <si>
     <t xml:space="preserve">w6_namesexage </t>
   </si>
   <si>
-    <t xml:space="preserve">higher_earner_education </t>
-  </si>
-  <si>
-    <t xml:space="preserve">higher_earner_occupation_prev </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q51_help_3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">q50_help_3 </t>
-  </si>
-  <si>
     <t xml:space="preserve">q41 </t>
   </si>
   <si>
@@ -3953,9 +3701,6 @@
     <t xml:space="preserve">q39 </t>
   </si>
   <si>
-    <t xml:space="preserve">q26_filter_8 </t>
-  </si>
-  <si>
     <t xml:space="preserve">q_panel </t>
   </si>
   <si>
@@ -4004,9 +3749,6 @@
     <t xml:space="preserve">qrorigin_rec </t>
   </si>
   <si>
-    <t>check_to_remove</t>
-  </si>
-  <si>
     <t xml:space="preserve">qmktsize_refused_to_answer </t>
   </si>
   <si>
@@ -4260,6 +4002,18 @@
   </si>
   <si>
     <t>cnt_bar_rest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk_nations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">uk02inc </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w7_namesexage </t>
+  </si>
+  <si>
+    <t xml:space="preserve">w8_namesexage </t>
   </si>
 </sst>
 </file>
@@ -4627,12 +4381,12 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>1372</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>1373</v>
+        <v>1287</v>
       </c>
     </row>
   </sheetData>
@@ -26761,7 +26515,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1C5985-D720-4533-B6F5-A2816F80F2F5}">
   <dimension ref="A1:B418"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A294" workbookViewId="0">
+    <sheetView topLeftCell="A294" workbookViewId="0">
       <selection activeCell="B336" sqref="B336"/>
     </sheetView>
   </sheetViews>
@@ -27648,7 +27402,7 @@
         <v>402</v>
       </c>
       <c r="B110" t="s">
-        <v>1374</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.45">
@@ -27656,7 +27410,7 @@
         <v>102</v>
       </c>
       <c r="B111" t="s">
-        <v>1375</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.45">
@@ -27664,7 +27418,7 @@
         <v>103</v>
       </c>
       <c r="B112" t="s">
-        <v>1376</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
@@ -28656,7 +28410,7 @@
         <v>192</v>
       </c>
       <c r="B236" t="s">
-        <v>1379</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.45">
@@ -28664,7 +28418,7 @@
         <v>1018</v>
       </c>
       <c r="B237" t="s">
-        <v>1399</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.45">
@@ -28672,7 +28426,7 @@
         <v>1019</v>
       </c>
       <c r="B238" t="s">
-        <v>1380</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.45">
@@ -28680,7 +28434,7 @@
         <v>1020</v>
       </c>
       <c r="B239" t="s">
-        <v>1381</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.45">
@@ -28688,7 +28442,7 @@
         <v>1021</v>
       </c>
       <c r="B240" t="s">
-        <v>1382</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.45">
@@ -28696,7 +28450,7 @@
         <v>1022</v>
       </c>
       <c r="B241" t="s">
-        <v>1383</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.45">
@@ -28704,7 +28458,7 @@
         <v>1023</v>
       </c>
       <c r="B242" t="s">
-        <v>1384</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.45">
@@ -28712,7 +28466,7 @@
         <v>1024</v>
       </c>
       <c r="B243" t="s">
-        <v>1385</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.45">
@@ -28720,7 +28474,7 @@
         <v>1025</v>
       </c>
       <c r="B244" t="s">
-        <v>1386</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.45">
@@ -28728,7 +28482,7 @@
         <v>1026</v>
       </c>
       <c r="B245" t="s">
-        <v>1387</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.45">
@@ -28880,7 +28634,7 @@
         <v>1046</v>
       </c>
       <c r="B264" t="s">
-        <v>1377</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.45">
@@ -28888,7 +28642,7 @@
         <v>1047</v>
       </c>
       <c r="B265" t="s">
-        <v>1378</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.45">
@@ -29056,7 +28810,7 @@
         <v>197</v>
       </c>
       <c r="B286" t="s">
-        <v>1403</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.45">
@@ -29240,7 +28994,7 @@
         <v>451</v>
       </c>
       <c r="B309" t="s">
-        <v>1401</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.45">
@@ -29272,7 +29026,7 @@
         <v>455</v>
       </c>
       <c r="B313" t="s">
-        <v>1389</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.45">
@@ -29368,7 +29122,7 @@
         <v>466</v>
       </c>
       <c r="B325" t="s">
-        <v>1388</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.45">
@@ -29456,7 +29210,7 @@
         <v>477</v>
       </c>
       <c r="B336" t="s">
-        <v>1404</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.45">
@@ -30979,7 +30733,7 @@
         <v>413</v>
       </c>
       <c r="B106" t="s">
-        <v>1400</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.45">
@@ -31011,7 +30765,7 @@
         <v>417</v>
       </c>
       <c r="B110" t="s">
-        <v>1390</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.45">
@@ -31019,7 +30773,7 @@
         <v>418</v>
       </c>
       <c r="B111" t="s">
-        <v>1391</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.45">
@@ -31027,7 +30781,7 @@
         <v>419</v>
       </c>
       <c r="B112" t="s">
-        <v>1392</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
@@ -31035,7 +30789,7 @@
         <v>420</v>
       </c>
       <c r="B113" t="s">
-        <v>1386</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
@@ -31043,7 +30797,7 @@
         <v>421</v>
       </c>
       <c r="B114" t="s">
-        <v>1393</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
@@ -31051,7 +30805,7 @@
         <v>422</v>
       </c>
       <c r="B115" t="s">
-        <v>1394</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.45">
@@ -31059,7 +30813,7 @@
         <v>423</v>
       </c>
       <c r="B116" t="s">
-        <v>1395</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
@@ -31067,7 +30821,7 @@
         <v>424</v>
       </c>
       <c r="B117" t="s">
-        <v>1380</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
@@ -31075,7 +30829,7 @@
         <v>425</v>
       </c>
       <c r="B118" t="s">
-        <v>1396</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.45">
@@ -31083,7 +30837,7 @@
         <v>426</v>
       </c>
       <c r="B119" t="s">
-        <v>1397</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
@@ -31091,7 +30845,7 @@
         <v>427</v>
       </c>
       <c r="B120" t="s">
-        <v>1398</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
@@ -31275,7 +31029,7 @@
         <v>451</v>
       </c>
       <c r="B143" t="s">
-        <v>1401</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
@@ -31307,7 +31061,7 @@
         <v>455</v>
       </c>
       <c r="B147" t="s">
-        <v>1389</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.45">
@@ -31403,7 +31157,7 @@
         <v>466</v>
       </c>
       <c r="B159" t="s">
-        <v>1388</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.45">
@@ -31491,7 +31245,7 @@
         <v>477</v>
       </c>
       <c r="B170" t="s">
-        <v>1404</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.45">
@@ -32469,7 +32223,7 @@
         <v>1169</v>
       </c>
       <c r="D19" t="s">
-        <v>1402</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
@@ -32483,7 +32237,7 @@
         <v>1162</v>
       </c>
       <c r="D20" t="s">
-        <v>1402</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
@@ -35033,10 +34787,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB4B1FA-6628-4BA2-9F29-B27CBB154F46}">
-  <dimension ref="A1:B111"/>
+  <dimension ref="A1:A120"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -35044,840 +34798,609 @@
     <col min="1" max="1" width="36.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>1371</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1319</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>1305</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1171</v>
       </c>
-      <c r="B3" t="s">
-        <v>1175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>1307</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1176</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1177</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>1235</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1178</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>1172</v>
       </c>
-      <c r="B7" t="s">
-        <v>1179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>1279</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>1308</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>1241</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1173</v>
       </c>
-      <c r="B11" t="s">
-        <v>1183</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>1303</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>1304</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1185</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>1174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>1236</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A80" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
         <v>1274</v>
       </c>
-      <c r="B14" t="s">
-        <v>1186</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A82" t="s">
         <v>1275</v>
       </c>
-      <c r="B15" t="s">
-        <v>1187</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>1310</v>
-      </c>
-      <c r="B16" t="s">
-        <v>1188</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>1311</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1189</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>1312</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>1313</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1192</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>1315</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1193</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>1316</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1202</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>1317</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1203</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>1318</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1204</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>1205</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>1201</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1232</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>1194</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1254</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>1195</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1229</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>1240</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>1242</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1207</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>1243</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1255</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>1244</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1263</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>1197</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1264</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>1233</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1265</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
         <v>1276</v>
       </c>
-      <c r="B35" t="s">
-        <v>1266</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A84" t="s">
         <v>1277</v>
       </c>
-      <c r="B36" t="s">
-        <v>1268</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
         <v>1278</v>
       </c>
-      <c r="B37" t="s">
-        <v>1256</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A86" t="s">
+        <v>1279</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A88" t="s">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A90" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
         <v>1284</v>
       </c>
-      <c r="B38" t="s">
-        <v>1269</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>1289</v>
-      </c>
-      <c r="B39" t="s">
-        <v>1270</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>1294</v>
-      </c>
-      <c r="B40" t="s">
-        <v>1271</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>1320</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1272</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>1321</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1257</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>1322</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>1323</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1281</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>1324</v>
-      </c>
-      <c r="B45" t="s">
-        <v>1282</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>1325</v>
-      </c>
-      <c r="B46" t="s">
-        <v>1283</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>1326</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>1327</v>
-      </c>
-      <c r="B48" t="s">
-        <v>1285</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>1328</v>
-      </c>
-      <c r="B49" t="s">
-        <v>1286</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>1329</v>
-      </c>
-      <c r="B50" t="s">
-        <v>1287</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>1330</v>
-      </c>
-      <c r="B51" t="s">
-        <v>1288</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
-        <v>1331</v>
-      </c>
-      <c r="B52" t="s">
-        <v>1259</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>1332</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1290</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
-        <v>1333</v>
-      </c>
-      <c r="B54" t="s">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>1334</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1292</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>1335</v>
-      </c>
-      <c r="B56" t="s">
-        <v>1293</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>1336</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>1337</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1261</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>1338</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1267</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>1340</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
-        <v>1341</v>
-      </c>
-      <c r="B62" t="s">
-        <v>1231</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
-        <v>1342</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1208</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
-        <v>1343</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1209</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>1344</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1210</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>1345</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1211</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
-        <v>1346</v>
-      </c>
-      <c r="B67" t="s">
-        <v>1212</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1213</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>1348</v>
-      </c>
-      <c r="B69" t="s">
-        <v>1214</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
-        <v>1349</v>
-      </c>
-      <c r="B70" t="s">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
-        <v>1350</v>
-      </c>
-      <c r="B71" t="s">
-        <v>1216</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A72" t="s">
-        <v>1351</v>
-      </c>
-      <c r="B72" t="s">
-        <v>1217</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>1352</v>
-      </c>
-      <c r="B73" t="s">
-        <v>1218</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>1353</v>
-      </c>
-      <c r="B74" t="s">
-        <v>1219</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>1354</v>
-      </c>
-      <c r="B75" t="s">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
-        <v>1355</v>
-      </c>
-      <c r="B76" t="s">
-        <v>1221</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>1356</v>
-      </c>
-      <c r="B77" t="s">
-        <v>1222</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
-        <v>1357</v>
-      </c>
-      <c r="B78" t="s">
-        <v>1223</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
-        <v>1358</v>
-      </c>
-      <c r="B79" t="s">
-        <v>1224</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
-        <v>1359</v>
-      </c>
-      <c r="B80" t="s">
-        <v>1302</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>1360</v>
-      </c>
-      <c r="B81" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
-        <v>1361</v>
-      </c>
-      <c r="B82" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
-        <v>1362</v>
-      </c>
-      <c r="B83" t="s">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A84" t="s">
-        <v>1363</v>
-      </c>
-      <c r="B84" t="s">
-        <v>1299</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A85" t="s">
-        <v>1364</v>
-      </c>
-      <c r="B85" t="s">
-        <v>1198</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A86" t="s">
-        <v>1365</v>
-      </c>
-      <c r="B86" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A87" t="s">
-        <v>1366</v>
-      </c>
-      <c r="B87" t="s">
-        <v>1306</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A88" t="s">
-        <v>1367</v>
-      </c>
-      <c r="B88" t="s">
-        <v>1298</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A89" t="s">
-        <v>1368</v>
-      </c>
-      <c r="B89" t="s">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A90" t="s">
-        <v>1369</v>
-      </c>
-      <c r="B90" t="s">
-        <v>1297</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A91" t="s">
-        <v>1370</v>
-      </c>
-      <c r="B91" t="s">
-        <v>1236</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.45">
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>229</v>
       </c>
-      <c r="B92" t="s">
-        <v>1237</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B93" t="s">
-        <v>1225</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B94" t="s">
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B95" t="s">
-        <v>1227</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B96" t="s">
-        <v>1238</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B97" t="s">
-        <v>1239</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B98" t="s">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B99" t="s">
-        <v>1273</v>
-      </c>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B100" t="s">
-        <v>1245</v>
-      </c>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B101" t="s">
-        <v>1246</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B102" t="s">
-        <v>1247</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B103" t="s">
-        <v>1248</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B104" t="s">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B105" t="s">
-        <v>1251</v>
-      </c>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B106" t="s">
-        <v>1252</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B107" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B108" t="s">
-        <v>1249</v>
-      </c>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B109" t="s">
-        <v>1295</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B110" t="s">
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A94" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A96" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A98" t="s">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A102" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>1178</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A104" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A106" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A108" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A110" t="s">
         <v>1196</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B111" t="s">
-        <v>1296</v>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A112" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A114" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A115" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A116" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>1203</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A118" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A119" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A120" t="s">
+        <v>1322</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A484">
-    <sortCondition ref="A2:A484"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A481">
+    <sortCondition ref="A2:A481"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update for new vaccine variables
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,23 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB67827-4EC8-4D13-8FB6-4030E13FE351}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA60583-4088-470E-8BCD-B761A1D7456A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="3" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="1851" yWindow="1851" windowWidth="24686" windowHeight="13149" activeTab="1" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
-    <sheet name="All_vars" sheetId="1" r:id="rId2"/>
-    <sheet name="survey_1" sheetId="2" r:id="rId3"/>
-    <sheet name="survey_2" sheetId="3" r:id="rId4"/>
+    <sheet name="survey_2" sheetId="3" r:id="rId2"/>
+    <sheet name="All_vars" sheetId="1" r:id="rId3"/>
+    <sheet name="survey_1" sheetId="2" r:id="rId4"/>
     <sheet name="locations" sheetId="5" r:id="rId5"/>
     <sheet name="oldsheet_v2" sheetId="4" r:id="rId6"/>
     <sheet name="remove_vars" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">All_vars!$A$1:$K$650</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">survey_1!$A$1:$G$423</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">survey_2!$A$1:$B$262</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">All_vars!$A$1:$K$650</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">survey_1!$A$1:$G$423</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">survey_2!$A$1:$B$258</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2859" uniqueCount="1324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2907" uniqueCount="1372">
   <si>
     <t>vars</t>
   </si>
@@ -4017,6 +4017,150 @@
   </si>
   <si>
     <t>part_covid_test_recent</t>
+  </si>
+  <si>
+    <t>qxx1</t>
+  </si>
+  <si>
+    <t>qxx2</t>
+  </si>
+  <si>
+    <t>qzz1</t>
+  </si>
+  <si>
+    <t>qzz2</t>
+  </si>
+  <si>
+    <t>qxx3_scale_1_codes</t>
+  </si>
+  <si>
+    <t>qxx3_scale_2_codes</t>
+  </si>
+  <si>
+    <t>qxx3_scale_3_codes</t>
+  </si>
+  <si>
+    <t>qxx3_scale_4_codes</t>
+  </si>
+  <si>
+    <t>qxx3_scale_1</t>
+  </si>
+  <si>
+    <t>qxx3_scale_2</t>
+  </si>
+  <si>
+    <t>qxx3_scale_3</t>
+  </si>
+  <si>
+    <t>qxx3_scale_4</t>
+  </si>
+  <si>
+    <t>part_vacc</t>
+  </si>
+  <si>
+    <t>part_vacc_doses</t>
+  </si>
+  <si>
+    <t>part_vacc_dose1_date</t>
+  </si>
+  <si>
+    <t>part_vacc_dose2_date</t>
+  </si>
+  <si>
+    <t>part_vacc_dose3_date</t>
+  </si>
+  <si>
+    <t>part_vacc_dose4_date</t>
+  </si>
+  <si>
+    <t>qxx3_scale_5_codes</t>
+  </si>
+  <si>
+    <t>part_vacc_dose5_date</t>
+  </si>
+  <si>
+    <t>qxx3_scale_5</t>
+  </si>
+  <si>
+    <t>part_vacc_dose1_date_dk</t>
+  </si>
+  <si>
+    <t>part_vacc_dose2_date_dk</t>
+  </si>
+  <si>
+    <t>part_vacc_dose3_date_dk</t>
+  </si>
+  <si>
+    <t>part_vacc_dose4_date_dk</t>
+  </si>
+  <si>
+    <t>part_vacc_dose5_date_dk</t>
+  </si>
+  <si>
+    <t>part_vacc_newdose</t>
+  </si>
+  <si>
+    <t>part_vacc_newdose_doses</t>
+  </si>
+  <si>
+    <t>qzz3_scale_1</t>
+  </si>
+  <si>
+    <t>qzz3_scale_2</t>
+  </si>
+  <si>
+    <t>qzz3_scale_3</t>
+  </si>
+  <si>
+    <t>qzz3_scale_4</t>
+  </si>
+  <si>
+    <t>qzz3_scale_5</t>
+  </si>
+  <si>
+    <t>qzz3_scale_1_codes</t>
+  </si>
+  <si>
+    <t>qzz3_scale_2_codes</t>
+  </si>
+  <si>
+    <t>qzz3_scale_3_codes</t>
+  </si>
+  <si>
+    <t>qzz3_scale_4_codes</t>
+  </si>
+  <si>
+    <t>qzz3_scale_5_codes</t>
+  </si>
+  <si>
+    <t>part_vacc_newdose_dose1_date</t>
+  </si>
+  <si>
+    <t>part_vacc_newdose_dose2_date</t>
+  </si>
+  <si>
+    <t>part_vacc_newdose_dose3_date</t>
+  </si>
+  <si>
+    <t>part_vacc_newdose_dose4_date</t>
+  </si>
+  <si>
+    <t>part_vacc_newdose_dose5_date</t>
+  </si>
+  <si>
+    <t>part_vacc_newdose_dose1_date_dk</t>
+  </si>
+  <si>
+    <t>part_vacc_newdose_dose2_date_dk</t>
+  </si>
+  <si>
+    <t>part_vacc_newdose_dose3_date_dk</t>
+  </si>
+  <si>
+    <t>part_vacc_newdose_dose4_date_dk</t>
+  </si>
+  <si>
+    <t>part_vacc_newdose_dose5_date_dk</t>
   </si>
 </sst>
 </file>
@@ -4398,6 +4542,2263 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6804872F-908E-4576-8C9F-D057085582A0}">
+  <dimension ref="A1:B280"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
+      <selection activeCell="A271" sqref="A271:C280"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="21.69140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>556</v>
+      </c>
+      <c r="B1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>310</v>
+      </c>
+      <c r="B6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>312</v>
+      </c>
+      <c r="B8" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>314</v>
+      </c>
+      <c r="B9" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>315</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>317</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>318</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>319</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>320</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>321</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>323</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>324</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>325</v>
+      </c>
+      <c r="B19" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>326</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>327</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>328</v>
+      </c>
+      <c r="B22" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>329</v>
+      </c>
+      <c r="B23" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>330</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>331</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>332</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>333</v>
+      </c>
+      <c r="B27" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>334</v>
+      </c>
+      <c r="B28" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>335</v>
+      </c>
+      <c r="B29" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>337</v>
+      </c>
+      <c r="B30" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>339</v>
+      </c>
+      <c r="B31" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>341</v>
+      </c>
+      <c r="B32" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>343</v>
+      </c>
+      <c r="B33" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>345</v>
+      </c>
+      <c r="B34" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
+        <v>347</v>
+      </c>
+      <c r="B35" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>348</v>
+      </c>
+      <c r="B36" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>349</v>
+      </c>
+      <c r="B37" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>355</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>350</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>351</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>352</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
+        <v>353</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>354</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>360</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>356</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
+        <v>357</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>358</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>359</v>
+      </c>
+      <c r="B48" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>365</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>361</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>362</v>
+      </c>
+      <c r="B51" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>363</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>364</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>370</v>
+      </c>
+      <c r="B54" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A55" t="s">
+        <v>366</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>367</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>368</v>
+      </c>
+      <c r="B57" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>369</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>375</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>371</v>
+      </c>
+      <c r="B60" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
+        <v>372</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
+        <v>373</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
+        <v>374</v>
+      </c>
+      <c r="B63" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
+        <v>376</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A65" t="s">
+        <v>377</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A66" t="s">
+        <v>378</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A67" t="s">
+        <v>379</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
+        <v>380</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A69" t="s">
+        <v>381</v>
+      </c>
+      <c r="B69" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A70" t="s">
+        <v>382</v>
+      </c>
+      <c r="B70" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A71" t="s">
+        <v>383</v>
+      </c>
+      <c r="B71" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A72" t="s">
+        <v>384</v>
+      </c>
+      <c r="B72" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
+        <v>599</v>
+      </c>
+      <c r="B73" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
+        <v>601</v>
+      </c>
+      <c r="B74" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
+        <v>603</v>
+      </c>
+      <c r="B75" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
+        <v>605</v>
+      </c>
+      <c r="B76" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A77" t="s">
+        <v>385</v>
+      </c>
+      <c r="B77" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A78" t="s">
+        <v>386</v>
+      </c>
+      <c r="B78" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A79" t="s">
+        <v>387</v>
+      </c>
+      <c r="B79" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
+        <v>388</v>
+      </c>
+      <c r="B80" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
+        <v>389</v>
+      </c>
+      <c r="B81" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A82" t="s">
+        <v>390</v>
+      </c>
+      <c r="B82" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
+        <v>391</v>
+      </c>
+      <c r="B83" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
+        <v>392</v>
+      </c>
+      <c r="B84" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
+        <v>393</v>
+      </c>
+      <c r="B85" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
+        <v>394</v>
+      </c>
+      <c r="B86" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A87" t="s">
+        <v>395</v>
+      </c>
+      <c r="B87" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
+        <v>396</v>
+      </c>
+      <c r="B88" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A89" t="s">
+        <v>397</v>
+      </c>
+      <c r="B89" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A90" t="s">
+        <v>398</v>
+      </c>
+      <c r="B90" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
+        <v>399</v>
+      </c>
+      <c r="B91" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
+        <v>400</v>
+      </c>
+      <c r="B92" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A93" t="s">
+        <v>401</v>
+      </c>
+      <c r="B93" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A94" t="s">
+        <v>402</v>
+      </c>
+      <c r="B94" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
+        <v>403</v>
+      </c>
+      <c r="B95" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
+        <v>405</v>
+      </c>
+      <c r="B96" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A97" t="s">
+        <v>406</v>
+      </c>
+      <c r="B97" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A98" t="s">
+        <v>1081</v>
+      </c>
+      <c r="B98" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B99" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A100" t="s">
+        <v>407</v>
+      </c>
+      <c r="B100" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A101" t="s">
+        <v>408</v>
+      </c>
+      <c r="B101" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A102" t="s">
+        <v>409</v>
+      </c>
+      <c r="B102" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A103" t="s">
+        <v>410</v>
+      </c>
+      <c r="B103" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A104" t="s">
+        <v>411</v>
+      </c>
+      <c r="B104" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A105" t="s">
+        <v>412</v>
+      </c>
+      <c r="B105" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A106" t="s">
+        <v>413</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A107" t="s">
+        <v>414</v>
+      </c>
+      <c r="B107" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A108" t="s">
+        <v>415</v>
+      </c>
+      <c r="B108" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A109" t="s">
+        <v>416</v>
+      </c>
+      <c r="B109" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A110" t="s">
+        <v>417</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A111" t="s">
+        <v>418</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A112" t="s">
+        <v>419</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A113" t="s">
+        <v>420</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A114" t="s">
+        <v>421</v>
+      </c>
+      <c r="B114" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A115" t="s">
+        <v>422</v>
+      </c>
+      <c r="B115" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A116" t="s">
+        <v>423</v>
+      </c>
+      <c r="B116" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A117" t="s">
+        <v>424</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A118" t="s">
+        <v>425</v>
+      </c>
+      <c r="B118" t="s">
+        <v>1310</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A119" t="s">
+        <v>426</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A120" t="s">
+        <v>427</v>
+      </c>
+      <c r="B120" t="s">
+        <v>1312</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
+        <v>428</v>
+      </c>
+      <c r="B121" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A122" t="s">
+        <v>429</v>
+      </c>
+      <c r="B122" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A123" t="s">
+        <v>431</v>
+      </c>
+      <c r="B123" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A124" t="s">
+        <v>432</v>
+      </c>
+      <c r="B124" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A125" t="s">
+        <v>433</v>
+      </c>
+      <c r="B125" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A126" t="s">
+        <v>434</v>
+      </c>
+      <c r="B126" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A127" t="s">
+        <v>435</v>
+      </c>
+      <c r="B127" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A128" t="s">
+        <v>436</v>
+      </c>
+      <c r="B128" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A129" t="s">
+        <v>437</v>
+      </c>
+      <c r="B129" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A130" t="s">
+        <v>438</v>
+      </c>
+      <c r="B130" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A131" t="s">
+        <v>439</v>
+      </c>
+      <c r="B131" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A132" t="s">
+        <v>440</v>
+      </c>
+      <c r="B132" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A133" t="s">
+        <v>441</v>
+      </c>
+      <c r="B133" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A134" t="s">
+        <v>442</v>
+      </c>
+      <c r="B134" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A135" t="s">
+        <v>443</v>
+      </c>
+      <c r="B135" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A136" t="s">
+        <v>444</v>
+      </c>
+      <c r="B136" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A137" t="s">
+        <v>445</v>
+      </c>
+      <c r="B137" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A138" t="s">
+        <v>446</v>
+      </c>
+      <c r="B138" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A139" t="s">
+        <v>447</v>
+      </c>
+      <c r="B139" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A140" t="s">
+        <v>448</v>
+      </c>
+      <c r="B140" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A141" t="s">
+        <v>449</v>
+      </c>
+      <c r="B141" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A142" t="s">
+        <v>450</v>
+      </c>
+      <c r="B142" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A143" t="s">
+        <v>451</v>
+      </c>
+      <c r="B143" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A144" t="s">
+        <v>452</v>
+      </c>
+      <c r="B144" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A145" t="s">
+        <v>453</v>
+      </c>
+      <c r="B145" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A146" t="s">
+        <v>454</v>
+      </c>
+      <c r="B146" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A147" t="s">
+        <v>455</v>
+      </c>
+      <c r="B147" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A148" t="s">
+        <v>456</v>
+      </c>
+      <c r="B148" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A149" t="s">
+        <v>457</v>
+      </c>
+      <c r="B149" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A150" t="s">
+        <v>458</v>
+      </c>
+      <c r="B150" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A151" t="s">
+        <v>459</v>
+      </c>
+      <c r="B151" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A152" t="s">
+        <v>460</v>
+      </c>
+      <c r="B152" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A153" t="s">
+        <v>461</v>
+      </c>
+      <c r="B153" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A154" t="s">
+        <v>462</v>
+      </c>
+      <c r="B154" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A155" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B155" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A156" t="s">
+        <v>463</v>
+      </c>
+      <c r="B156" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A157" t="s">
+        <v>464</v>
+      </c>
+      <c r="B157" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A158" t="s">
+        <v>465</v>
+      </c>
+      <c r="B158" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A159" t="s">
+        <v>466</v>
+      </c>
+      <c r="B159" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A160" t="s">
+        <v>467</v>
+      </c>
+      <c r="B160" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A161" t="s">
+        <v>468</v>
+      </c>
+      <c r="B161" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A162" t="s">
+        <v>469</v>
+      </c>
+      <c r="B162" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A163" t="s">
+        <v>470</v>
+      </c>
+      <c r="B163" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A164" t="s">
+        <v>471</v>
+      </c>
+      <c r="B164" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A165" t="s">
+        <v>472</v>
+      </c>
+      <c r="B165" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A166" t="s">
+        <v>473</v>
+      </c>
+      <c r="B166" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A167" t="s">
+        <v>474</v>
+      </c>
+      <c r="B167" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A168" t="s">
+        <v>475</v>
+      </c>
+      <c r="B168" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A169" t="s">
+        <v>476</v>
+      </c>
+      <c r="B169" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A170" t="s">
+        <v>477</v>
+      </c>
+      <c r="B170" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A171" t="s">
+        <v>479</v>
+      </c>
+      <c r="B171" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A172" t="s">
+        <v>480</v>
+      </c>
+      <c r="B172" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A173" t="s">
+        <v>481</v>
+      </c>
+      <c r="B173" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A174" t="s">
+        <v>482</v>
+      </c>
+      <c r="B174" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A175" t="s">
+        <v>483</v>
+      </c>
+      <c r="B175" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A176" t="s">
+        <v>484</v>
+      </c>
+      <c r="B176" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A177" t="s">
+        <v>485</v>
+      </c>
+      <c r="B177" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A178" t="s">
+        <v>486</v>
+      </c>
+      <c r="B178" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A179" t="s">
+        <v>487</v>
+      </c>
+      <c r="B179" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A180" t="s">
+        <v>488</v>
+      </c>
+      <c r="B180" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A181" t="s">
+        <v>489</v>
+      </c>
+      <c r="B181" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A182" t="s">
+        <v>490</v>
+      </c>
+      <c r="B182" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A183" t="s">
+        <v>491</v>
+      </c>
+      <c r="B183" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A184" t="s">
+        <v>492</v>
+      </c>
+      <c r="B184" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A185" t="s">
+        <v>493</v>
+      </c>
+      <c r="B185" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A186" t="s">
+        <v>982</v>
+      </c>
+      <c r="B186" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A187" t="s">
+        <v>983</v>
+      </c>
+      <c r="B187" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A188" t="s">
+        <v>984</v>
+      </c>
+      <c r="B188" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A189" t="s">
+        <v>495</v>
+      </c>
+      <c r="B189" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A190" t="s">
+        <v>986</v>
+      </c>
+      <c r="B190" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A191" t="s">
+        <v>987</v>
+      </c>
+      <c r="B191" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A192" t="s">
+        <v>988</v>
+      </c>
+      <c r="B192" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A193" t="s">
+        <v>497</v>
+      </c>
+      <c r="B193" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A194" t="s">
+        <v>990</v>
+      </c>
+      <c r="B194" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A195" t="s">
+        <v>991</v>
+      </c>
+      <c r="B195" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A196" t="s">
+        <v>992</v>
+      </c>
+      <c r="B196" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A197" t="s">
+        <v>499</v>
+      </c>
+      <c r="B197" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A198" t="s">
+        <v>500</v>
+      </c>
+      <c r="B198" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A199" t="s">
+        <v>501</v>
+      </c>
+      <c r="B199" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A200" t="s">
+        <v>502</v>
+      </c>
+      <c r="B200" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A201" t="s">
+        <v>503</v>
+      </c>
+      <c r="B201" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A202" t="s">
+        <v>504</v>
+      </c>
+      <c r="B202" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A203" t="s">
+        <v>512</v>
+      </c>
+      <c r="B203" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A204" t="s">
+        <v>505</v>
+      </c>
+      <c r="B204" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A205" t="s">
+        <v>506</v>
+      </c>
+      <c r="B205" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A206" t="s">
+        <v>507</v>
+      </c>
+      <c r="B206" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A207" t="s">
+        <v>508</v>
+      </c>
+      <c r="B207" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A208" t="s">
+        <v>509</v>
+      </c>
+      <c r="B208" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A209" t="s">
+        <v>510</v>
+      </c>
+      <c r="B209" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A210" t="s">
+        <v>511</v>
+      </c>
+      <c r="B210" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A211" t="s">
+        <v>517</v>
+      </c>
+      <c r="B211" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A212" t="s">
+        <v>513</v>
+      </c>
+      <c r="B212" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A213" t="s">
+        <v>514</v>
+      </c>
+      <c r="B213" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A214" t="s">
+        <v>515</v>
+      </c>
+      <c r="B214" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A215" t="s">
+        <v>518</v>
+      </c>
+      <c r="B215" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A216" t="s">
+        <v>519</v>
+      </c>
+      <c r="B216" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A217" t="s">
+        <v>521</v>
+      </c>
+      <c r="B217" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A218" t="s">
+        <v>520</v>
+      </c>
+      <c r="B218" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A219" t="s">
+        <v>522</v>
+      </c>
+      <c r="B219" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A220" t="s">
+        <v>523</v>
+      </c>
+      <c r="B220" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A221" t="s">
+        <v>524</v>
+      </c>
+      <c r="B221" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A222" t="s">
+        <v>525</v>
+      </c>
+      <c r="B222" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A223" t="s">
+        <v>526</v>
+      </c>
+      <c r="B223" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A224" t="s">
+        <v>527</v>
+      </c>
+      <c r="B224" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A225" t="s">
+        <v>528</v>
+      </c>
+      <c r="B225" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A226" t="s">
+        <v>529</v>
+      </c>
+      <c r="B226" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A227" t="s">
+        <v>530</v>
+      </c>
+      <c r="B227" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A228" t="s">
+        <v>531</v>
+      </c>
+      <c r="B228" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A229" t="s">
+        <v>532</v>
+      </c>
+      <c r="B229" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A230" t="s">
+        <v>533</v>
+      </c>
+      <c r="B230" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A231" t="s">
+        <v>534</v>
+      </c>
+      <c r="B231" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A232" t="s">
+        <v>536</v>
+      </c>
+      <c r="B232" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A233" t="s">
+        <v>538</v>
+      </c>
+      <c r="B233" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A234" t="s">
+        <v>540</v>
+      </c>
+      <c r="B234" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A235" t="s">
+        <v>542</v>
+      </c>
+      <c r="B235" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A236" t="s">
+        <v>290</v>
+      </c>
+      <c r="B236" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A237" t="s">
+        <v>291</v>
+      </c>
+      <c r="B237" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A238" t="s">
+        <v>292</v>
+      </c>
+      <c r="B238" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A239" t="s">
+        <v>293</v>
+      </c>
+      <c r="B239" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A240" t="s">
+        <v>545</v>
+      </c>
+      <c r="B240" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A241" t="s">
+        <v>294</v>
+      </c>
+      <c r="B241" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A242" t="s">
+        <v>295</v>
+      </c>
+      <c r="B242" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A243" t="s">
+        <v>296</v>
+      </c>
+      <c r="B243" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A244" t="s">
+        <v>297</v>
+      </c>
+      <c r="B244" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A245" t="s">
+        <v>547</v>
+      </c>
+      <c r="B245" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A246" t="s">
+        <v>298</v>
+      </c>
+      <c r="B246" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A247" t="s">
+        <v>548</v>
+      </c>
+      <c r="B247" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A248" t="s">
+        <v>299</v>
+      </c>
+      <c r="B248" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A249" t="s">
+        <v>300</v>
+      </c>
+      <c r="B249" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A250" t="s">
+        <v>549</v>
+      </c>
+      <c r="B250" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A251" t="s">
+        <v>550</v>
+      </c>
+      <c r="B251" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A252" t="s">
+        <v>551</v>
+      </c>
+      <c r="B252" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A253" t="s">
+        <v>552</v>
+      </c>
+      <c r="B253" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A254" t="s">
+        <v>553</v>
+      </c>
+      <c r="B254" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A255" t="s">
+        <v>554</v>
+      </c>
+      <c r="B255" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A256" t="s">
+        <v>555</v>
+      </c>
+      <c r="B256" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A257" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B257" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A258" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B258" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A259" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B259" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A260" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B260" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A261" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B261" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A262" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B262" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A263" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B263" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A264" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B264" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A265" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B265" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A266" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B266" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A267" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B267" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A268" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B268" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A269" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B269" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A270" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B270" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A271" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B271" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A272" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B272" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A273" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B273" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A274" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B274" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A275" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B275" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A276" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B276" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A277" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B277" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A278" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B278" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A279" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B279" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A280" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B280" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59DB8823-33FC-4C68-8AB1-65768017318F}">
   <dimension ref="A1:K650"/>
   <sheetViews>
@@ -26514,11 +28915,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1C5985-D720-4533-B6F5-A2816F80F2F5}">
   <dimension ref="A1:B418"/>
   <sheetViews>
-    <sheetView topLeftCell="A294" workbookViewId="0">
+    <sheetView topLeftCell="A385" workbookViewId="0">
       <selection activeCell="B336" sqref="B336"/>
     </sheetView>
   </sheetViews>
@@ -29878,2071 +32279,6 @@
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6804872F-908E-4576-8C9F-D057085582A0}">
-  <dimension ref="A1:B256"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="21.69140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>556</v>
-      </c>
-      <c r="B1" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>306</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>307</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B4" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>309</v>
-      </c>
-      <c r="B5" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>310</v>
-      </c>
-      <c r="B6" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>311</v>
-      </c>
-      <c r="B7" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>312</v>
-      </c>
-      <c r="B8" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>314</v>
-      </c>
-      <c r="B9" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>315</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>317</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>318</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>319</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>320</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>321</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B16" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>323</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>324</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>325</v>
-      </c>
-      <c r="B19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>326</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>327</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
-        <v>328</v>
-      </c>
-      <c r="B22" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>329</v>
-      </c>
-      <c r="B23" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
-        <v>330</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>331</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>332</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A27" t="s">
-        <v>333</v>
-      </c>
-      <c r="B27" t="s">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A28" t="s">
-        <v>334</v>
-      </c>
-      <c r="B28" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A29" t="s">
-        <v>335</v>
-      </c>
-      <c r="B29" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A30" t="s">
-        <v>337</v>
-      </c>
-      <c r="B30" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A31" t="s">
-        <v>339</v>
-      </c>
-      <c r="B31" t="s">
-        <v>927</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A32" t="s">
-        <v>341</v>
-      </c>
-      <c r="B32" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A33" t="s">
-        <v>343</v>
-      </c>
-      <c r="B33" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A34" t="s">
-        <v>345</v>
-      </c>
-      <c r="B34" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A35" t="s">
-        <v>347</v>
-      </c>
-      <c r="B35" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A36" t="s">
-        <v>348</v>
-      </c>
-      <c r="B36" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A37" t="s">
-        <v>349</v>
-      </c>
-      <c r="B37" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A38" t="s">
-        <v>355</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A39" t="s">
-        <v>350</v>
-      </c>
-      <c r="B39" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A40" t="s">
-        <v>351</v>
-      </c>
-      <c r="B40" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A41" t="s">
-        <v>352</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A42" t="s">
-        <v>353</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A43" t="s">
-        <v>354</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A44" t="s">
-        <v>360</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A45" t="s">
-        <v>356</v>
-      </c>
-      <c r="B45" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A46" t="s">
-        <v>357</v>
-      </c>
-      <c r="B46" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A47" t="s">
-        <v>358</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A48" t="s">
-        <v>359</v>
-      </c>
-      <c r="B48" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A49" t="s">
-        <v>365</v>
-      </c>
-      <c r="B49" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A50" t="s">
-        <v>361</v>
-      </c>
-      <c r="B50" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A51" t="s">
-        <v>362</v>
-      </c>
-      <c r="B51" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A52" t="s">
-        <v>363</v>
-      </c>
-      <c r="B52" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A53" t="s">
-        <v>364</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A54" t="s">
-        <v>370</v>
-      </c>
-      <c r="B54" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
-        <v>366</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
-        <v>367</v>
-      </c>
-      <c r="B56" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
-        <v>368</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
-        <v>369</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
-        <v>375</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A60" t="s">
-        <v>371</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
-        <v>372</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
-        <v>373</v>
-      </c>
-      <c r="B62" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
-        <v>374</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A64" t="s">
-        <v>376</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A65" t="s">
-        <v>377</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A66" t="s">
-        <v>378</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A67" t="s">
-        <v>379</v>
-      </c>
-      <c r="B67" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A68" t="s">
-        <v>380</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A69" t="s">
-        <v>381</v>
-      </c>
-      <c r="B69" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A70" t="s">
-        <v>382</v>
-      </c>
-      <c r="B70" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A71" t="s">
-        <v>383</v>
-      </c>
-      <c r="B71" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A72" t="s">
-        <v>384</v>
-      </c>
-      <c r="B72" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A73" t="s">
-        <v>599</v>
-      </c>
-      <c r="B73" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A74" t="s">
-        <v>601</v>
-      </c>
-      <c r="B74" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A75" t="s">
-        <v>603</v>
-      </c>
-      <c r="B75" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A76" t="s">
-        <v>605</v>
-      </c>
-      <c r="B76" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A77" t="s">
-        <v>385</v>
-      </c>
-      <c r="B77" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A78" t="s">
-        <v>386</v>
-      </c>
-      <c r="B78" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A79" t="s">
-        <v>387</v>
-      </c>
-      <c r="B79" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A80" t="s">
-        <v>388</v>
-      </c>
-      <c r="B80" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A81" t="s">
-        <v>389</v>
-      </c>
-      <c r="B81" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A82" t="s">
-        <v>390</v>
-      </c>
-      <c r="B82" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A83" t="s">
-        <v>391</v>
-      </c>
-      <c r="B83" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A84" t="s">
-        <v>392</v>
-      </c>
-      <c r="B84" t="s">
-        <v>1086</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A85" t="s">
-        <v>393</v>
-      </c>
-      <c r="B85" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A86" t="s">
-        <v>394</v>
-      </c>
-      <c r="B86" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A87" t="s">
-        <v>395</v>
-      </c>
-      <c r="B87" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A88" t="s">
-        <v>396</v>
-      </c>
-      <c r="B88" t="s">
-        <v>939</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A89" t="s">
-        <v>397</v>
-      </c>
-      <c r="B89" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A90" t="s">
-        <v>398</v>
-      </c>
-      <c r="B90" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A91" t="s">
-        <v>399</v>
-      </c>
-      <c r="B91" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A92" t="s">
-        <v>400</v>
-      </c>
-      <c r="B92" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A93" t="s">
-        <v>401</v>
-      </c>
-      <c r="B93" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A94" t="s">
-        <v>402</v>
-      </c>
-      <c r="B94" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A95" t="s">
-        <v>403</v>
-      </c>
-      <c r="B95" t="s">
-        <v>945</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A96" t="s">
-        <v>405</v>
-      </c>
-      <c r="B96" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A97" t="s">
-        <v>406</v>
-      </c>
-      <c r="B97" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A98" t="s">
-        <v>1081</v>
-      </c>
-      <c r="B98" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A99" t="s">
-        <v>1082</v>
-      </c>
-      <c r="B99" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A100" t="s">
-        <v>407</v>
-      </c>
-      <c r="B100" t="s">
-        <v>947</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A101" t="s">
-        <v>408</v>
-      </c>
-      <c r="B101" t="s">
-        <v>948</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A102" t="s">
-        <v>409</v>
-      </c>
-      <c r="B102" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A103" t="s">
-        <v>410</v>
-      </c>
-      <c r="B103" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A104" t="s">
-        <v>411</v>
-      </c>
-      <c r="B104" t="s">
-        <v>951</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A105" t="s">
-        <v>412</v>
-      </c>
-      <c r="B105" t="s">
-        <v>952</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A106" t="s">
-        <v>413</v>
-      </c>
-      <c r="B106" t="s">
-        <v>1314</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A107" t="s">
-        <v>414</v>
-      </c>
-      <c r="B107" t="s">
-        <v>954</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A108" t="s">
-        <v>415</v>
-      </c>
-      <c r="B108" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A109" t="s">
-        <v>416</v>
-      </c>
-      <c r="B109" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A110" t="s">
-        <v>417</v>
-      </c>
-      <c r="B110" t="s">
-        <v>1304</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A111" t="s">
-        <v>418</v>
-      </c>
-      <c r="B111" t="s">
-        <v>1305</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A112" t="s">
-        <v>419</v>
-      </c>
-      <c r="B112" t="s">
-        <v>1306</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A113" t="s">
-        <v>420</v>
-      </c>
-      <c r="B113" t="s">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A114" t="s">
-        <v>421</v>
-      </c>
-      <c r="B114" t="s">
-        <v>1307</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A115" t="s">
-        <v>422</v>
-      </c>
-      <c r="B115" t="s">
-        <v>1308</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A116" t="s">
-        <v>423</v>
-      </c>
-      <c r="B116" t="s">
-        <v>1309</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A117" t="s">
-        <v>424</v>
-      </c>
-      <c r="B117" t="s">
-        <v>1294</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A118" t="s">
-        <v>425</v>
-      </c>
-      <c r="B118" t="s">
-        <v>1310</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A119" t="s">
-        <v>426</v>
-      </c>
-      <c r="B119" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A120" t="s">
-        <v>427</v>
-      </c>
-      <c r="B120" t="s">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A121" t="s">
-        <v>428</v>
-      </c>
-      <c r="B121" t="s">
-        <v>796</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A122" t="s">
-        <v>429</v>
-      </c>
-      <c r="B122" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A123" t="s">
-        <v>431</v>
-      </c>
-      <c r="B123" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A124" t="s">
-        <v>432</v>
-      </c>
-      <c r="B124" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A125" t="s">
-        <v>433</v>
-      </c>
-      <c r="B125" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A126" t="s">
-        <v>434</v>
-      </c>
-      <c r="B126" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A127" t="s">
-        <v>435</v>
-      </c>
-      <c r="B127" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A128" t="s">
-        <v>436</v>
-      </c>
-      <c r="B128" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A129" t="s">
-        <v>437</v>
-      </c>
-      <c r="B129" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A130" t="s">
-        <v>438</v>
-      </c>
-      <c r="B130" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A131" t="s">
-        <v>439</v>
-      </c>
-      <c r="B131" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A132" t="s">
-        <v>440</v>
-      </c>
-      <c r="B132" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A133" t="s">
-        <v>441</v>
-      </c>
-      <c r="B133" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A134" t="s">
-        <v>442</v>
-      </c>
-      <c r="B134" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A135" t="s">
-        <v>443</v>
-      </c>
-      <c r="B135" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A136" t="s">
-        <v>444</v>
-      </c>
-      <c r="B136" t="s">
-        <v>821</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A137" t="s">
-        <v>445</v>
-      </c>
-      <c r="B137" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A138" t="s">
-        <v>446</v>
-      </c>
-      <c r="B138" t="s">
-        <v>823</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A139" t="s">
-        <v>447</v>
-      </c>
-      <c r="B139" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A140" t="s">
-        <v>448</v>
-      </c>
-      <c r="B140" t="s">
-        <v>825</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A141" t="s">
-        <v>449</v>
-      </c>
-      <c r="B141" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A142" t="s">
-        <v>450</v>
-      </c>
-      <c r="B142" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A143" t="s">
-        <v>451</v>
-      </c>
-      <c r="B143" t="s">
-        <v>1315</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A144" t="s">
-        <v>452</v>
-      </c>
-      <c r="B144" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A145" t="s">
-        <v>453</v>
-      </c>
-      <c r="B145" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A146" t="s">
-        <v>454</v>
-      </c>
-      <c r="B146" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A147" t="s">
-        <v>455</v>
-      </c>
-      <c r="B147" t="s">
-        <v>1303</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A148" t="s">
-        <v>456</v>
-      </c>
-      <c r="B148" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A149" t="s">
-        <v>457</v>
-      </c>
-      <c r="B149" t="s">
-        <v>837</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A150" t="s">
-        <v>458</v>
-      </c>
-      <c r="B150" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A151" t="s">
-        <v>459</v>
-      </c>
-      <c r="B151" t="s">
-        <v>838</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A152" t="s">
-        <v>460</v>
-      </c>
-      <c r="B152" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A153" t="s">
-        <v>461</v>
-      </c>
-      <c r="B153" t="s">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A154" t="s">
-        <v>462</v>
-      </c>
-      <c r="B154" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A155" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B155" t="s">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A156" t="s">
-        <v>463</v>
-      </c>
-      <c r="B156" t="s">
-        <v>843</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A157" t="s">
-        <v>464</v>
-      </c>
-      <c r="B157" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A158" t="s">
-        <v>465</v>
-      </c>
-      <c r="B158" t="s">
-        <v>845</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A159" t="s">
-        <v>466</v>
-      </c>
-      <c r="B159" t="s">
-        <v>1302</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A160" t="s">
-        <v>467</v>
-      </c>
-      <c r="B160" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A161" t="s">
-        <v>468</v>
-      </c>
-      <c r="B161" t="s">
-        <v>857</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A162" t="s">
-        <v>469</v>
-      </c>
-      <c r="B162" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A163" t="s">
-        <v>470</v>
-      </c>
-      <c r="B163" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A164" t="s">
-        <v>471</v>
-      </c>
-      <c r="B164" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A165" t="s">
-        <v>472</v>
-      </c>
-      <c r="B165" t="s">
-        <v>850</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A166" t="s">
-        <v>473</v>
-      </c>
-      <c r="B166" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A167" t="s">
-        <v>474</v>
-      </c>
-      <c r="B167" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A168" t="s">
-        <v>475</v>
-      </c>
-      <c r="B168" t="s">
-        <v>853</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A169" t="s">
-        <v>476</v>
-      </c>
-      <c r="B169" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A170" t="s">
-        <v>477</v>
-      </c>
-      <c r="B170" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A171" t="s">
-        <v>479</v>
-      </c>
-      <c r="B171" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A172" t="s">
-        <v>480</v>
-      </c>
-      <c r="B172" t="s">
-        <v>863</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A173" t="s">
-        <v>481</v>
-      </c>
-      <c r="B173" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A174" t="s">
-        <v>482</v>
-      </c>
-      <c r="B174" t="s">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A175" t="s">
-        <v>483</v>
-      </c>
-      <c r="B175" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A176" t="s">
-        <v>484</v>
-      </c>
-      <c r="B176" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A177" t="s">
-        <v>485</v>
-      </c>
-      <c r="B177" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A178" t="s">
-        <v>486</v>
-      </c>
-      <c r="B178" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A179" t="s">
-        <v>487</v>
-      </c>
-      <c r="B179" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A180" t="s">
-        <v>488</v>
-      </c>
-      <c r="B180" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A181" t="s">
-        <v>489</v>
-      </c>
-      <c r="B181" t="s">
-        <v>1095</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A182" t="s">
-        <v>490</v>
-      </c>
-      <c r="B182" t="s">
-        <v>1096</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A183" t="s">
-        <v>491</v>
-      </c>
-      <c r="B183" t="s">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A184" t="s">
-        <v>492</v>
-      </c>
-      <c r="B184" t="s">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A185" t="s">
-        <v>493</v>
-      </c>
-      <c r="B185" t="s">
-        <v>1099</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A186" t="s">
-        <v>982</v>
-      </c>
-      <c r="B186" t="s">
-        <v>883</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A187" t="s">
-        <v>983</v>
-      </c>
-      <c r="B187" t="s">
-        <v>889</v>
-      </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A188" t="s">
-        <v>984</v>
-      </c>
-      <c r="B188" t="s">
-        <v>895</v>
-      </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A189" t="s">
-        <v>495</v>
-      </c>
-      <c r="B189" t="s">
-        <v>985</v>
-      </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A190" t="s">
-        <v>986</v>
-      </c>
-      <c r="B190" t="s">
-        <v>885</v>
-      </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A191" t="s">
-        <v>987</v>
-      </c>
-      <c r="B191" t="s">
-        <v>891</v>
-      </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A192" t="s">
-        <v>988</v>
-      </c>
-      <c r="B192" t="s">
-        <v>897</v>
-      </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A193" t="s">
-        <v>497</v>
-      </c>
-      <c r="B193" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A194" t="s">
-        <v>990</v>
-      </c>
-      <c r="B194" t="s">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A195" t="s">
-        <v>991</v>
-      </c>
-      <c r="B195" t="s">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A196" t="s">
-        <v>992</v>
-      </c>
-      <c r="B196" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A197" t="s">
-        <v>499</v>
-      </c>
-      <c r="B197" t="s">
-        <v>993</v>
-      </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A198" t="s">
-        <v>500</v>
-      </c>
-      <c r="B198" t="s">
-        <v>994</v>
-      </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A199" t="s">
-        <v>501</v>
-      </c>
-      <c r="B199" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A200" t="s">
-        <v>502</v>
-      </c>
-      <c r="B200" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A201" t="s">
-        <v>503</v>
-      </c>
-      <c r="B201" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A202" t="s">
-        <v>504</v>
-      </c>
-      <c r="B202" t="s">
-        <v>995</v>
-      </c>
-    </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A203" t="s">
-        <v>512</v>
-      </c>
-      <c r="B203" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A204" t="s">
-        <v>505</v>
-      </c>
-      <c r="B204" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A205" t="s">
-        <v>506</v>
-      </c>
-      <c r="B205" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A206" t="s">
-        <v>507</v>
-      </c>
-      <c r="B206" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A207" t="s">
-        <v>508</v>
-      </c>
-      <c r="B207" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A208" t="s">
-        <v>509</v>
-      </c>
-      <c r="B208" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A209" t="s">
-        <v>510</v>
-      </c>
-      <c r="B209" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A210" t="s">
-        <v>511</v>
-      </c>
-      <c r="B210" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A211" t="s">
-        <v>517</v>
-      </c>
-      <c r="B211" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A212" t="s">
-        <v>513</v>
-      </c>
-      <c r="B212" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A213" t="s">
-        <v>514</v>
-      </c>
-      <c r="B213" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A214" t="s">
-        <v>515</v>
-      </c>
-      <c r="B214" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A215" t="s">
-        <v>518</v>
-      </c>
-      <c r="B215" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A216" t="s">
-        <v>519</v>
-      </c>
-      <c r="B216" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A217" t="s">
-        <v>521</v>
-      </c>
-      <c r="B217" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A218" t="s">
-        <v>520</v>
-      </c>
-      <c r="B218" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A219" t="s">
-        <v>522</v>
-      </c>
-      <c r="B219" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A220" t="s">
-        <v>523</v>
-      </c>
-      <c r="B220" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A221" t="s">
-        <v>524</v>
-      </c>
-      <c r="B221" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A222" t="s">
-        <v>525</v>
-      </c>
-      <c r="B222" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A223" t="s">
-        <v>526</v>
-      </c>
-      <c r="B223" t="s">
-        <v>996</v>
-      </c>
-    </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A224" t="s">
-        <v>527</v>
-      </c>
-      <c r="B224" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A225" t="s">
-        <v>528</v>
-      </c>
-      <c r="B225" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A226" t="s">
-        <v>529</v>
-      </c>
-      <c r="B226" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A227" t="s">
-        <v>530</v>
-      </c>
-      <c r="B227" t="s">
-        <v>997</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A228" t="s">
-        <v>531</v>
-      </c>
-      <c r="B228" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A229" t="s">
-        <v>532</v>
-      </c>
-      <c r="B229" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A230" t="s">
-        <v>533</v>
-      </c>
-      <c r="B230" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A231" t="s">
-        <v>534</v>
-      </c>
-      <c r="B231" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A232" t="s">
-        <v>536</v>
-      </c>
-      <c r="B232" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A233" t="s">
-        <v>538</v>
-      </c>
-      <c r="B233" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A234" t="s">
-        <v>540</v>
-      </c>
-      <c r="B234" t="s">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A235" t="s">
-        <v>542</v>
-      </c>
-      <c r="B235" t="s">
-        <v>1090</v>
-      </c>
-    </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A236" t="s">
-        <v>290</v>
-      </c>
-      <c r="B236" t="s">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A237" t="s">
-        <v>291</v>
-      </c>
-      <c r="B237" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A238" t="s">
-        <v>292</v>
-      </c>
-      <c r="B238" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A239" t="s">
-        <v>293</v>
-      </c>
-      <c r="B239" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A240" t="s">
-        <v>545</v>
-      </c>
-      <c r="B240" t="s">
-        <v>1001</v>
-      </c>
-    </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A241" t="s">
-        <v>294</v>
-      </c>
-      <c r="B241" t="s">
-        <v>1002</v>
-      </c>
-    </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A242" t="s">
-        <v>295</v>
-      </c>
-      <c r="B242" t="s">
-        <v>1003</v>
-      </c>
-    </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A243" t="s">
-        <v>296</v>
-      </c>
-      <c r="B243" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A244" t="s">
-        <v>297</v>
-      </c>
-      <c r="B244" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A245" t="s">
-        <v>547</v>
-      </c>
-      <c r="B245" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A246" t="s">
-        <v>298</v>
-      </c>
-      <c r="B246" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A247" t="s">
-        <v>548</v>
-      </c>
-      <c r="B247" t="s">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A248" t="s">
-        <v>299</v>
-      </c>
-      <c r="B248" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A249" t="s">
-        <v>300</v>
-      </c>
-      <c r="B249" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A250" t="s">
-        <v>549</v>
-      </c>
-      <c r="B250" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A251" t="s">
-        <v>550</v>
-      </c>
-      <c r="B251" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A252" t="s">
-        <v>551</v>
-      </c>
-      <c r="B252" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A253" t="s">
-        <v>552</v>
-      </c>
-      <c r="B253" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A254" t="s">
-        <v>553</v>
-      </c>
-      <c r="B254" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A255" t="s">
-        <v>554</v>
-      </c>
-      <c r="B255" t="s">
-        <v>1083</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A256" t="s">
-        <v>555</v>
-      </c>
-      <c r="B256" t="s">
-        <v>555</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update with new UK data Panel F wave 43 and new var names
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE27C3D-4E53-4D93-9663-F7296DEA74E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD34F7C-E2E4-4EC4-873C-5C4B879C742C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="15523" yWindow="994" windowWidth="16714" windowHeight="15052" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3790" uniqueCount="1344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3790" uniqueCount="1345">
   <si>
     <t>be01edu_me</t>
   </si>
@@ -4077,6 +4077,9 @@
   </si>
   <si>
     <t>Detail</t>
+  </si>
+  <si>
+    <t>hhm_symp_nausea</t>
   </si>
 </sst>
 </file>
@@ -15860,8 +15863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A651A7-E2A8-48DC-A289-3ADEDF80FEC9}">
   <dimension ref="A1:B298"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B298"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -16203,7 +16206,7 @@
         <v>49</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>507</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
@@ -18192,6 +18195,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
change multi contacts for V4 and V5
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD34F7C-E2E4-4EC4-873C-5C4B879C742C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD2188D-A9BE-40F6-A90A-F75E837AAE64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15523" yWindow="994" windowWidth="16714" windowHeight="15052" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="5640" yWindow="994" windowWidth="26597" windowHeight="15052" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3790" uniqueCount="1345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3784" uniqueCount="1339">
   <si>
     <t>be01edu_me</t>
   </si>
@@ -3776,15 +3776,9 @@
     <t>q79a_1_scale</t>
   </si>
   <si>
-    <t>multiple_contacts_under_12_work</t>
-  </si>
-  <si>
     <t>q79a_2_scale</t>
   </si>
   <si>
-    <t>multiple_contacts_12_17_work</t>
-  </si>
-  <si>
     <t>q79a_3_scale</t>
   </si>
   <si>
@@ -3803,15 +3797,9 @@
     <t>q80a_1_scale</t>
   </si>
   <si>
-    <t>multiple_contacts_under_12_school</t>
-  </si>
-  <si>
     <t>q80a_2_scale</t>
   </si>
   <si>
-    <t>multiple_contacts_12_17_school</t>
-  </si>
-  <si>
     <t>q80a_3_scale</t>
   </si>
   <si>
@@ -3830,13 +3818,7 @@
     <t>q81a_1_scale</t>
   </si>
   <si>
-    <t>multiple_contacts_under_12_other</t>
-  </si>
-  <si>
     <t>q81a_2_scale</t>
-  </si>
-  <si>
-    <t>multiple_contacts_12_17_other</t>
   </si>
   <si>
     <t>q81a_3_scale</t>
@@ -4459,66 +4441,66 @@
   <sheetData>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>1342</v>
+        <v>1336</v>
       </c>
       <c r="B3" t="s">
-        <v>1343</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>1328</v>
+        <v>1322</v>
       </c>
       <c r="B4" t="s">
-        <v>1335</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>1329</v>
+        <v>1323</v>
       </c>
       <c r="B5" t="s">
-        <v>1330</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>1331</v>
+        <v>1325</v>
       </c>
       <c r="B6" t="s">
-        <v>1334</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>1332</v>
+        <v>1326</v>
       </c>
       <c r="B7" t="s">
-        <v>1336</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>1333</v>
+        <v>1327</v>
       </c>
       <c r="B8" t="s">
-        <v>1337</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
-        <v>1338</v>
+        <v>1332</v>
       </c>
       <c r="B9" t="s">
-        <v>1339</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
-        <v>1340</v>
+        <v>1334</v>
       </c>
       <c r="B10" t="s">
-        <v>1341</v>
+        <v>1335</v>
       </c>
     </row>
   </sheetData>
@@ -7898,7 +7880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6804872F-908E-4576-8C9F-D057085582A0}">
   <dimension ref="A1:B418"/>
   <sheetViews>
-    <sheetView topLeftCell="A369" workbookViewId="0">
+    <sheetView topLeftCell="A327" workbookViewId="0">
       <selection activeCell="A418" sqref="A418"/>
     </sheetView>
   </sheetViews>
@@ -11264,8 +11246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2811056-AE3B-4304-B94A-E79692ED9D00}">
   <dimension ref="A1:B281"/>
   <sheetViews>
-    <sheetView topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="A281" sqref="A281"/>
+    <sheetView topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="B194" sqref="B194:B196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -13528,7 +13510,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837411D0-7592-4667-8DD0-A212016903E8}">
   <dimension ref="A1:B298"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="B172" sqref="B155:B172"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -14730,144 +14714,138 @@
       <c r="A155" s="3" t="s">
         <v>1242</v>
       </c>
-      <c r="B155" s="3" t="s">
-        <v>1243</v>
+      <c r="B155" s="4" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A156" s="3" t="s">
-        <v>1244</v>
-      </c>
-      <c r="B156" s="3" t="s">
-        <v>1245</v>
+        <v>1243</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A157" s="3" t="s">
-        <v>1246</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>772</v>
+        <v>1244</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>778</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A158" s="3" t="s">
-        <v>1247</v>
-      </c>
-      <c r="B158" s="2" t="s">
-        <v>778</v>
-      </c>
+        <v>1245</v>
+      </c>
+      <c r="B158" s="2"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A159" s="3" t="s">
         <v>402</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A160" s="3" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A161" s="3" t="s">
-        <v>1251</v>
-      </c>
-      <c r="B161" s="3" t="s">
-        <v>1252</v>
+        <v>1249</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A162" s="3" t="s">
-        <v>1253</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>1254</v>
+        <v>1250</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>774</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A163" s="3" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>774</v>
+        <v>1251</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>780</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A164" s="3" t="s">
-        <v>1256</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>780</v>
-      </c>
+        <v>1252</v>
+      </c>
+      <c r="B164" s="2"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A165" s="3" t="s">
         <v>403</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A166" s="3" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A167" s="3" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>1261</v>
+        <v>1256</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>770</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A168" s="3" t="s">
-        <v>1262</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>1263</v>
+        <v>1257</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>776</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A169" s="3" t="s">
-        <v>1264</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>776</v>
+        <v>1258</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>782</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A170" s="3" t="s">
-        <v>1265</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>782</v>
-      </c>
+        <v>1259</v>
+      </c>
+      <c r="B170" s="2"/>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A171" s="3" t="s">
         <v>404</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1266</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A172" s="3" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1268</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.4">
@@ -15451,7 +15429,7 @@
         <v>0</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>1269</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.4">
@@ -15475,7 +15453,7 @@
         <v>3</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>1270</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.4">
@@ -15483,7 +15461,7 @@
         <v>4</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>1271</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.4">
@@ -15499,7 +15477,7 @@
         <v>6</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>1272</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.4">
@@ -15507,7 +15485,7 @@
         <v>7</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>1273</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.4">
@@ -15515,7 +15493,7 @@
         <v>8</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>1274</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.4">
@@ -15523,7 +15501,7 @@
         <v>9</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>1275</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.4">
@@ -15531,12 +15509,12 @@
         <v>224</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>1276</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A258" s="2" t="s">
-        <v>1277</v>
+        <v>1271</v>
       </c>
       <c r="B258" s="2" t="s">
         <v>1143</v>
@@ -15544,7 +15522,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A259" s="2" t="s">
-        <v>1278</v>
+        <v>1272</v>
       </c>
       <c r="B259" s="2" t="s">
         <v>1163</v>
@@ -15552,7 +15530,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A260" s="2" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="B260" s="3" t="s">
         <v>834</v>
@@ -15560,23 +15538,23 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A261" s="2" t="s">
-        <v>1280</v>
+        <v>1274</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>1281</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A262" s="2" t="s">
-        <v>1282</v>
+        <v>1276</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>1283</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A263" s="2" t="s">
-        <v>1284</v>
+        <v>1278</v>
       </c>
       <c r="B263" s="2" t="s">
         <v>1144</v>
@@ -15584,7 +15562,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A264" s="2" t="s">
-        <v>1285</v>
+        <v>1279</v>
       </c>
       <c r="B264" s="2" t="s">
         <v>1145</v>
@@ -15592,7 +15570,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A265" s="2" t="s">
-        <v>1286</v>
+        <v>1280</v>
       </c>
       <c r="B265" s="2" t="s">
         <v>1146</v>
@@ -15600,7 +15578,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A266" s="2" t="s">
-        <v>1287</v>
+        <v>1281</v>
       </c>
       <c r="B266" s="2" t="s">
         <v>1147</v>
@@ -15608,7 +15586,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A267" s="2" t="s">
-        <v>1288</v>
+        <v>1282</v>
       </c>
       <c r="B267" s="2" t="s">
         <v>1148</v>
@@ -15616,7 +15594,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A268" s="2" t="s">
-        <v>1289</v>
+        <v>1283</v>
       </c>
       <c r="B268" s="2" t="s">
         <v>1149</v>
@@ -15624,7 +15602,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A269" s="2" t="s">
-        <v>1290</v>
+        <v>1284</v>
       </c>
       <c r="B269" s="2" t="s">
         <v>1150</v>
@@ -15632,7 +15610,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A270" s="2" t="s">
-        <v>1291</v>
+        <v>1285</v>
       </c>
       <c r="B270" s="2" t="s">
         <v>1151</v>
@@ -15643,87 +15621,87 @@
         <v>296</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>1292</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A273" s="2" t="s">
-        <v>1293</v>
+        <v>1287</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>1294</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A274" s="2" t="s">
-        <v>1295</v>
+        <v>1289</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>1296</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A275" s="2" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>1298</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A276" s="2" t="s">
-        <v>1299</v>
+        <v>1293</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>1300</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A277" s="2" t="s">
-        <v>1301</v>
+        <v>1295</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>1302</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A278" s="2" t="s">
-        <v>1303</v>
+        <v>1297</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>1304</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A279" s="2" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>1306</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A280" s="2" t="s">
-        <v>1307</v>
+        <v>1301</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>1308</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A281" s="2" t="s">
-        <v>1309</v>
+        <v>1303</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>1310</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A282" s="2" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>1312</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.4">
@@ -15752,10 +15730,10 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A286" s="2" t="s">
-        <v>1313</v>
+        <v>1307</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>1314</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.4">
@@ -15763,7 +15741,7 @@
         <v>359</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>1315</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.4">
@@ -15771,7 +15749,7 @@
         <v>362</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>1316</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.4">
@@ -15779,7 +15757,7 @@
         <v>363</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.4">
@@ -15787,7 +15765,7 @@
         <v>338</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.4">
@@ -15795,7 +15773,7 @@
         <v>192</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.4">
@@ -15803,7 +15781,7 @@
         <v>199</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>1320</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.4">
@@ -15811,7 +15789,7 @@
         <v>208</v>
       </c>
       <c r="B293" s="2" t="s">
-        <v>1321</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.4">
@@ -15819,7 +15797,7 @@
         <v>193</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>1322</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.4">
@@ -15827,7 +15805,7 @@
         <v>200</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>1323</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.4">
@@ -15835,7 +15813,7 @@
         <v>209</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>1324</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.4">
@@ -15843,15 +15821,15 @@
         <v>210</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>1325</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A298" s="2" t="s">
-        <v>1326</v>
+        <v>1320</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>1327</v>
+        <v>1321</v>
       </c>
     </row>
   </sheetData>
@@ -15863,11 +15841,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A651A7-E2A8-48DC-A289-3ADEDF80FEC9}">
   <dimension ref="A1:B298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="B155" sqref="B155:B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="22.84375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
@@ -16206,7 +16187,7 @@
         <v>49</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>1344</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.4">
@@ -17069,144 +17050,138 @@
       <c r="A155" s="5" t="s">
         <v>1242</v>
       </c>
-      <c r="B155" s="5" t="s">
-        <v>1243</v>
+      <c r="B155" s="4" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A156" s="5" t="s">
-        <v>1244</v>
-      </c>
-      <c r="B156" s="5" t="s">
-        <v>1245</v>
+        <v>1243</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>772</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A157" s="5" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>772</v>
+        <v>778</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A158" s="5" t="s">
-        <v>1247</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>778</v>
-      </c>
+        <v>1245</v>
+      </c>
+      <c r="B158" s="4"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A159" s="5" t="s">
         <v>402</v>
       </c>
       <c r="B159" s="5" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A160" s="5" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="B160" s="5" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A161" s="5" t="s">
-        <v>1251</v>
-      </c>
-      <c r="B161" s="5" t="s">
-        <v>1252</v>
+        <v>1249</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A162" s="5" t="s">
-        <v>1253</v>
-      </c>
-      <c r="B162" s="5" t="s">
-        <v>1254</v>
+        <v>1250</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>774</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A163" s="5" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>774</v>
+        <v>780</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A164" s="5" t="s">
-        <v>1256</v>
-      </c>
-      <c r="B164" s="4" t="s">
-        <v>780</v>
-      </c>
+        <v>1252</v>
+      </c>
+      <c r="B164" s="4"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A165" s="5" t="s">
         <v>403</v>
       </c>
       <c r="B165" s="5" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A166" s="5" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="B166" s="5" t="s">
-        <v>1259</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A167" s="5" t="s">
-        <v>1260</v>
-      </c>
-      <c r="B167" s="5" t="s">
-        <v>1261</v>
+        <v>1256</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>770</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A168" s="5" t="s">
-        <v>1262</v>
-      </c>
-      <c r="B168" s="5" t="s">
-        <v>1263</v>
+        <v>1257</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>776</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A169" s="5" t="s">
-        <v>1264</v>
+        <v>1258</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>776</v>
+        <v>782</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A170" s="5" t="s">
-        <v>1265</v>
-      </c>
-      <c r="B170" s="4" t="s">
-        <v>782</v>
-      </c>
+        <v>1259</v>
+      </c>
+      <c r="B170" s="4"/>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A171" s="5" t="s">
         <v>404</v>
       </c>
       <c r="B171" s="5" t="s">
-        <v>1266</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A172" s="5" t="s">
-        <v>1267</v>
+        <v>1261</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>1268</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.4">
@@ -17790,7 +17765,7 @@
         <v>0</v>
       </c>
       <c r="B247" s="5" t="s">
-        <v>1269</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.4">
@@ -17814,7 +17789,7 @@
         <v>3</v>
       </c>
       <c r="B250" s="5" t="s">
-        <v>1270</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.4">
@@ -17822,7 +17797,7 @@
         <v>4</v>
       </c>
       <c r="B251" s="5" t="s">
-        <v>1271</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.4">
@@ -17838,7 +17813,7 @@
         <v>6</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>1272</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.4">
@@ -17846,7 +17821,7 @@
         <v>7</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>1273</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.4">
@@ -17854,7 +17829,7 @@
         <v>8</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>1274</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.4">
@@ -17862,7 +17837,7 @@
         <v>9</v>
       </c>
       <c r="B256" s="5" t="s">
-        <v>1275</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.4">
@@ -17870,12 +17845,12 @@
         <v>224</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>1276</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A258" s="4" t="s">
-        <v>1277</v>
+        <v>1271</v>
       </c>
       <c r="B258" s="4" t="s">
         <v>1143</v>
@@ -17883,7 +17858,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A259" s="4" t="s">
-        <v>1278</v>
+        <v>1272</v>
       </c>
       <c r="B259" s="4" t="s">
         <v>1163</v>
@@ -17891,7 +17866,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A260" s="4" t="s">
-        <v>1279</v>
+        <v>1273</v>
       </c>
       <c r="B260" s="5" t="s">
         <v>834</v>
@@ -17899,23 +17874,23 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A261" s="4" t="s">
-        <v>1280</v>
+        <v>1274</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>1281</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A262" s="4" t="s">
-        <v>1282</v>
+        <v>1276</v>
       </c>
       <c r="B262" s="5" t="s">
-        <v>1283</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A263" s="4" t="s">
-        <v>1284</v>
+        <v>1278</v>
       </c>
       <c r="B263" s="4" t="s">
         <v>1144</v>
@@ -17923,7 +17898,7 @@
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A264" s="4" t="s">
-        <v>1285</v>
+        <v>1279</v>
       </c>
       <c r="B264" s="4" t="s">
         <v>1145</v>
@@ -17931,7 +17906,7 @@
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A265" s="4" t="s">
-        <v>1286</v>
+        <v>1280</v>
       </c>
       <c r="B265" s="4" t="s">
         <v>1146</v>
@@ -17939,7 +17914,7 @@
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A266" s="4" t="s">
-        <v>1287</v>
+        <v>1281</v>
       </c>
       <c r="B266" s="4" t="s">
         <v>1147</v>
@@ -17947,7 +17922,7 @@
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A267" s="4" t="s">
-        <v>1288</v>
+        <v>1282</v>
       </c>
       <c r="B267" s="4" t="s">
         <v>1148</v>
@@ -17955,7 +17930,7 @@
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A268" s="4" t="s">
-        <v>1289</v>
+        <v>1283</v>
       </c>
       <c r="B268" s="4" t="s">
         <v>1149</v>
@@ -17963,7 +17938,7 @@
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A269" s="4" t="s">
-        <v>1290</v>
+        <v>1284</v>
       </c>
       <c r="B269" s="4" t="s">
         <v>1150</v>
@@ -17971,7 +17946,7 @@
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A270" s="4" t="s">
-        <v>1291</v>
+        <v>1285</v>
       </c>
       <c r="B270" s="4" t="s">
         <v>1151</v>
@@ -17982,87 +17957,87 @@
         <v>296</v>
       </c>
       <c r="B272" s="4" t="s">
-        <v>1292</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A273" s="4" t="s">
-        <v>1293</v>
+        <v>1287</v>
       </c>
       <c r="B273" s="4" t="s">
-        <v>1294</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A274" s="4" t="s">
-        <v>1295</v>
+        <v>1289</v>
       </c>
       <c r="B274" s="4" t="s">
-        <v>1296</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A275" s="4" t="s">
-        <v>1297</v>
+        <v>1291</v>
       </c>
       <c r="B275" s="4" t="s">
-        <v>1298</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A276" s="4" t="s">
-        <v>1299</v>
+        <v>1293</v>
       </c>
       <c r="B276" s="4" t="s">
-        <v>1300</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A277" s="4" t="s">
-        <v>1301</v>
+        <v>1295</v>
       </c>
       <c r="B277" s="4" t="s">
-        <v>1302</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A278" s="4" t="s">
-        <v>1303</v>
+        <v>1297</v>
       </c>
       <c r="B278" s="4" t="s">
-        <v>1304</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A279" s="4" t="s">
-        <v>1305</v>
+        <v>1299</v>
       </c>
       <c r="B279" s="4" t="s">
-        <v>1306</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A280" s="4" t="s">
-        <v>1307</v>
+        <v>1301</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>1308</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A281" s="4" t="s">
-        <v>1309</v>
+        <v>1303</v>
       </c>
       <c r="B281" s="4" t="s">
-        <v>1310</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A282" s="4" t="s">
-        <v>1311</v>
+        <v>1305</v>
       </c>
       <c r="B282" s="4" t="s">
-        <v>1312</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.4">
@@ -18091,10 +18066,10 @@
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A286" s="4" t="s">
-        <v>1313</v>
+        <v>1307</v>
       </c>
       <c r="B286" s="4" t="s">
-        <v>1314</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.4">
@@ -18102,7 +18077,7 @@
         <v>359</v>
       </c>
       <c r="B287" s="4" t="s">
-        <v>1315</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.4">
@@ -18110,7 +18085,7 @@
         <v>362</v>
       </c>
       <c r="B288" s="4" t="s">
-        <v>1316</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.4">
@@ -18118,7 +18093,7 @@
         <v>363</v>
       </c>
       <c r="B289" s="4" t="s">
-        <v>1317</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.4">
@@ -18126,7 +18101,7 @@
         <v>338</v>
       </c>
       <c r="B290" s="5" t="s">
-        <v>1318</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.4">
@@ -18134,7 +18109,7 @@
         <v>192</v>
       </c>
       <c r="B291" s="4" t="s">
-        <v>1319</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.4">
@@ -18142,7 +18117,7 @@
         <v>199</v>
       </c>
       <c r="B292" s="4" t="s">
-        <v>1320</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.4">
@@ -18150,7 +18125,7 @@
         <v>208</v>
       </c>
       <c r="B293" s="4" t="s">
-        <v>1321</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.4">
@@ -18158,7 +18133,7 @@
         <v>193</v>
       </c>
       <c r="B294" s="4" t="s">
-        <v>1322</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.4">
@@ -18166,7 +18141,7 @@
         <v>200</v>
       </c>
       <c r="B295" s="4" t="s">
-        <v>1323</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.4">
@@ -18174,7 +18149,7 @@
         <v>209</v>
       </c>
       <c r="B296" s="4" t="s">
-        <v>1324</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.4">
@@ -18182,15 +18157,15 @@
         <v>210</v>
       </c>
       <c r="B297" s="4" t="s">
-        <v>1325</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A298" s="4" t="s">
-        <v>1326</v>
+        <v>1320</v>
       </c>
       <c r="B298" s="4" t="s">
-        <v>1327</v>
+        <v>1321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add duration to multiple contacts
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD2188D-A9BE-40F6-A90A-F75E837AAE64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161DC745-E582-407A-9713-3EDC3A54C9C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5640" yWindow="994" windowWidth="26597" windowHeight="15052" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="5640" yWindow="994" windowWidth="26597" windowHeight="15052" activeTab="3" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3784" uniqueCount="1339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3790" uniqueCount="1339">
   <si>
     <t>be01edu_me</t>
   </si>
@@ -11244,10 +11244,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2811056-AE3B-4304-B94A-E79692ED9D00}">
-  <dimension ref="A1:B281"/>
+  <dimension ref="A1:B284"/>
   <sheetViews>
-    <sheetView topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="B194" sqref="B194:B196"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200:B200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -12765,513 +12765,513 @@
         <v>845</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A190" s="1" t="s">
-        <v>846</v>
-      </c>
-      <c r="B190" s="1" t="s">
-        <v>768</v>
+    <row r="190" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A190" s="5" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B190" s="5" t="s">
+        <v>1248</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A191" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A192" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A193" s="1" t="s">
-        <v>403</v>
+        <v>848</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>849</v>
+        <v>780</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A194" s="1" t="s">
-        <v>850</v>
+        <v>403</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A195" s="1" t="s">
-        <v>851</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>776</v>
+        <v>849</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A195" s="5" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B195" s="5" t="s">
+        <v>1255</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A196" s="1" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>782</v>
+        <v>770</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A197" s="1" t="s">
-        <v>404</v>
+        <v>851</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>853</v>
+        <v>776</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A198" s="1" t="s">
-        <v>405</v>
+        <v>852</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>854</v>
+        <v>782</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A199" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A200" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>937</v>
+        <v>853</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A200" s="5" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B200" s="5" t="s">
+        <v>1262</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A201" s="1" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>461</v>
+        <v>854</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A202" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>855</v>
+        <v>937</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A203" s="1" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>468</v>
+        <v>937</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A204" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B204" s="1" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A205" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B205" s="1" t="s">
-        <v>478</v>
+        <v>855</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A206" s="1" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>479</v>
+        <v>468</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A207" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A208" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A209" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A210" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A211" s="1" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B211" s="1" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A212" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A213" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A214" s="1" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A215" s="1" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>470</v>
+        <v>484</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A216" s="1" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="B216" s="1" t="s">
-        <v>471</v>
+        <v>485</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A217" s="1" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="B217" s="1" t="s">
-        <v>472</v>
+        <v>486</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A218" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>488</v>
+        <v>470</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A219" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A220" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A221" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>475</v>
+        <v>488</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A222" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A223" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>856</v>
+        <v>474</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A224" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>458</v>
+        <v>475</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A225" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>459</v>
+        <v>476</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A226" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>457</v>
+        <v>856</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A227" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>857</v>
+        <v>458</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A228" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>436</v>
+        <v>459</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A229" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>437</v>
+        <v>457</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A230" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>460</v>
+        <v>857</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A231" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>462</v>
+        <v>436</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A232" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>463</v>
+        <v>437</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A233" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A234" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>858</v>
+        <v>462</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A235" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>942</v>
+        <v>463</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A236" s="1" t="s">
-        <v>211</v>
+        <v>441</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>859</v>
+        <v>464</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A237" s="1" t="s">
-        <v>212</v>
+        <v>442</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>212</v>
+        <v>858</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A238" s="1" t="s">
-        <v>213</v>
+        <v>443</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>213</v>
+        <v>942</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A239" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>214</v>
+        <v>859</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A240" s="1" t="s">
-        <v>445</v>
+        <v>212</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>860</v>
+        <v>212</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A241" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>861</v>
+        <v>213</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A242" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>862</v>
+        <v>214</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A243" s="1" t="s">
-        <v>217</v>
+        <v>445</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A244" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>937</v>
+        <v>861</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A245" s="1" t="s">
-        <v>446</v>
+        <v>216</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>446</v>
+        <v>862</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A246" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A247" s="1" t="s">
-        <v>447</v>
+        <v>218</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>865</v>
+        <v>937</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A248" s="1" t="s">
-        <v>220</v>
+        <v>446</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>866</v>
+        <v>446</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A249" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A250" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>937</v>
+        <v>865</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A251" s="1" t="s">
-        <v>449</v>
+        <v>220</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>937</v>
+        <v>866</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A252" s="1" t="s">
-        <v>450</v>
+        <v>221</v>
       </c>
       <c r="B252" s="1" t="s">
-        <v>937</v>
+        <v>867</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A253" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="B253" s="1" t="s">
         <v>937</v>
@@ -13279,7 +13279,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A254" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>937</v>
@@ -13287,7 +13287,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A255" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>937</v>
@@ -13295,209 +13295,233 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A256" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="B256" s="1" t="s">
-        <v>454</v>
+        <v>937</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A257" s="1" t="s">
-        <v>1174</v>
+        <v>452</v>
       </c>
       <c r="B257" s="1" t="s">
-        <v>1186</v>
+        <v>937</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A258" s="1" t="s">
-        <v>1175</v>
+        <v>453</v>
       </c>
       <c r="B258" s="1" t="s">
-        <v>1187</v>
+        <v>937</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A259" s="1" t="s">
-        <v>1182</v>
+        <v>454</v>
       </c>
       <c r="B259" s="1" t="s">
-        <v>1188</v>
+        <v>454</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A260" s="1" t="s">
-        <v>1183</v>
+        <v>1174</v>
       </c>
       <c r="B260" s="1" t="s">
-        <v>1189</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A261" s="1" t="s">
-        <v>1184</v>
+        <v>1175</v>
       </c>
       <c r="B261" s="1" t="s">
-        <v>1190</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A262" s="1" t="s">
-        <v>1185</v>
+        <v>1182</v>
       </c>
       <c r="B262" s="1" t="s">
-        <v>1191</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A263" s="1" t="s">
-        <v>1194</v>
+        <v>1183</v>
       </c>
       <c r="B263" s="1" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A264" s="1" t="s">
-        <v>1178</v>
+        <v>1184</v>
       </c>
       <c r="B264" s="1" t="s">
-        <v>1195</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A265" s="1" t="s">
-        <v>1179</v>
+        <v>1185</v>
       </c>
       <c r="B265" s="1" t="s">
-        <v>1196</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A266" s="1" t="s">
-        <v>1180</v>
+        <v>1194</v>
       </c>
       <c r="B266" s="1" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A267" s="1" t="s">
-        <v>1181</v>
+        <v>1178</v>
       </c>
       <c r="B267" s="1" t="s">
-        <v>1198</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A268" s="1" t="s">
-        <v>1192</v>
+        <v>1179</v>
       </c>
       <c r="B268" s="1" t="s">
-        <v>1199</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A269" s="1" t="s">
-        <v>1176</v>
+        <v>1180</v>
       </c>
       <c r="B269" s="1" t="s">
-        <v>1200</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A270" s="1" t="s">
-        <v>1177</v>
+        <v>1181</v>
       </c>
       <c r="B270" s="1" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A271" s="1" t="s">
-        <v>1202</v>
+        <v>1192</v>
       </c>
       <c r="B271" s="1" t="s">
-        <v>1212</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A272" s="1" t="s">
-        <v>1203</v>
+        <v>1176</v>
       </c>
       <c r="B272" s="1" t="s">
-        <v>1213</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A273" s="1" t="s">
-        <v>1204</v>
+        <v>1177</v>
       </c>
       <c r="B273" s="1" t="s">
-        <v>1214</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A274" s="1" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="B274" s="1" t="s">
-        <v>1215</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A275" s="1" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="B275" s="1" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A276" s="1" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="B276" s="1" t="s">
-        <v>1217</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A277" s="1" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="B277" s="1" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A278" s="1" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>1219</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A279" s="1" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="B279" s="1" t="s">
-        <v>1220</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A280" s="1" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>1221</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A281" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A282" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A283" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A284" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="B281" s="1" t="s">
+      <c r="B284" s="1" t="s">
         <v>465</v>
       </c>
     </row>
@@ -13511,7 +13535,7 @@
   <dimension ref="A1:B298"/>
   <sheetViews>
     <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="B172" sqref="B155:B172"/>
+      <selection activeCell="A172" sqref="A172:B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -15841,8 +15865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A651A7-E2A8-48DC-A289-3ADEDF80FEC9}">
   <dimension ref="A1:B298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="B155" sqref="B155:B172"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A160" sqref="A159:B160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
add group1/group2 and variable v4 cleaning (be/nl)
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/codebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D028939E-CC50-6F46-ADED-91FEEC8FA596}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BD650B-0384-6B48-A685-A0A8A3F48AE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="1000" windowWidth="26600" windowHeight="15060" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="2200" yWindow="1120" windowWidth="26600" windowHeight="15060" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
     <sheet name="survey_1" sheetId="2" r:id="rId2"/>
     <sheet name="survey_2" sheetId="3" r:id="rId3"/>
     <sheet name="survey_3" sheetId="8" r:id="rId4"/>
-    <sheet name="survey_4" sheetId="10" r:id="rId5"/>
-    <sheet name="survey_5" sheetId="9" r:id="rId6"/>
-    <sheet name="locations" sheetId="5" r:id="rId7"/>
-    <sheet name="remove_vars" sheetId="6" r:id="rId8"/>
+    <sheet name="survey_4_be" sheetId="10" r:id="rId5"/>
+    <sheet name="survey_4_nl" sheetId="11" r:id="rId6"/>
+    <sheet name="survey_5" sheetId="9" r:id="rId7"/>
+    <sheet name="locations" sheetId="5" r:id="rId8"/>
+    <sheet name="remove_vars" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">survey_1!$A$1:$G$423</definedName>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3812" uniqueCount="1362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4425" uniqueCount="1372">
   <si>
     <t>be01edu_me</t>
   </si>
@@ -4131,6 +4132,36 @@
   </si>
   <si>
     <t>destdregion</t>
+  </si>
+  <si>
+    <t>multiple_contacts_child_12_17_work</t>
+  </si>
+  <si>
+    <t>multiple_contacts_child_0_11_work</t>
+  </si>
+  <si>
+    <t>multiple_contacts_child_12_17_school</t>
+  </si>
+  <si>
+    <t>multiple_contacts_child_0_11_school</t>
+  </si>
+  <si>
+    <t>multiple_contacts_child_0_11_other</t>
+  </si>
+  <si>
+    <t>multiple_contacts_child_12_17_other</t>
+  </si>
+  <si>
+    <t>part_public_transport_other_text</t>
+  </si>
+  <si>
+    <t>q68a</t>
+  </si>
+  <si>
+    <t>elevated_risk_group</t>
+  </si>
+  <si>
+    <t>part_elevated_risk</t>
   </si>
 </sst>
 </file>
@@ -4583,7 +4614,7 @@
   <dimension ref="A1:B418"/>
   <sheetViews>
     <sheetView topLeftCell="A403" workbookViewId="0">
-      <selection activeCell="B405" sqref="B405"/>
+      <selection activeCell="B421" sqref="B421"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7949,8 +7980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6804872F-908E-4576-8C9F-D057085582A0}">
   <dimension ref="A1:B418"/>
   <sheetViews>
-    <sheetView topLeftCell="A327" workbookViewId="0">
-      <selection activeCell="A418" sqref="A418"/>
+    <sheetView topLeftCell="A346" workbookViewId="0">
+      <selection activeCell="A362" sqref="A362"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11315,8 +11346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2811056-AE3B-4304-B94A-E79692ED9D00}">
   <dimension ref="A1:B284"/>
   <sheetViews>
-    <sheetView topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="A200" sqref="A200:B200"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13601,13 +13632,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{837411D0-7592-4667-8DD0-A212016903E8}">
-  <dimension ref="A1:B298"/>
+  <dimension ref="A1:B314"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="A172" sqref="A172:B172"/>
+    <sheetView topLeftCell="A266" zoomScale="91" workbookViewId="0">
+      <selection activeCell="A283" sqref="A283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.33203125" customWidth="1"/>
+    <col min="2" max="2" width="32.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
@@ -14808,7 +14843,7 @@
         <v>1242</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>766</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
@@ -14816,7 +14851,7 @@
         <v>1243</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>772</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
@@ -14824,14 +14859,16 @@
         <v>1244</v>
       </c>
       <c r="B157" s="4" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
         <v>1245</v>
       </c>
-      <c r="B158" s="2"/>
+      <c r="B158" s="4" t="s">
+        <v>778</v>
+      </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
@@ -14854,7 +14891,7 @@
         <v>1249</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>768</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
@@ -14862,7 +14899,7 @@
         <v>1250</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>774</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
@@ -14870,14 +14907,16 @@
         <v>1251</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
         <v>1252</v>
       </c>
-      <c r="B164" s="2"/>
+      <c r="B164" s="4" t="s">
+        <v>780</v>
+      </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
@@ -14900,15 +14939,15 @@
         <v>1256</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>770</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>1257</v>
       </c>
-      <c r="B168" s="4" t="s">
-        <v>776</v>
+      <c r="B168" t="s">
+        <v>1367</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
@@ -14916,14 +14955,16 @@
         <v>1258</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>1259</v>
       </c>
-      <c r="B170" s="2"/>
+      <c r="B170" s="4" t="s">
+        <v>782</v>
+      </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
@@ -15924,6 +15965,69 @@
       <c r="B298" s="2" t="s">
         <v>1321</v>
       </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A299" s="5"/>
+      <c r="B299" s="4"/>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A300" s="5"/>
+      <c r="B300" s="4"/>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B301" s="4"/>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A302" s="5"/>
+      <c r="B302" s="4"/>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A303" s="5"/>
+      <c r="B303" s="5"/>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A304" s="5"/>
+      <c r="B304" s="5"/>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A305" s="5"/>
+      <c r="B305" s="4"/>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A306" s="5"/>
+      <c r="B306" s="4"/>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A307" s="5"/>
+      <c r="B307" s="4"/>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A308" s="5"/>
+      <c r="B308" s="4"/>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A309" s="5"/>
+      <c r="B309" s="5"/>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A310" s="5"/>
+      <c r="B310" s="5"/>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A311" s="5"/>
+      <c r="B311" s="4"/>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A312" s="5"/>
+      <c r="B312" s="4"/>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A313" s="5"/>
+      <c r="B313" s="4"/>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A314" s="5"/>
+      <c r="B314" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15931,11 +16035,2476 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01158CBA-7E67-C246-925F-8A45600A7C89}">
+  <dimension ref="A1:B306"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
+      <selection activeCell="A298" sqref="A298:XFD298"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>1371</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="4" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="4" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="4" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="4" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="4" t="s">
+        <v>935</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>1154</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="B120" s="4" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="B123" s="4" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="B125" s="4" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="5" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="5" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="B128" s="4" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="B129" s="4" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="B130" s="4" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B131" s="4" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="B132" s="4" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B133" s="4" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="5" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B134" s="5" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B136" s="4" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="4" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="4" t="s">
+        <v>881</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="4" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="4" t="s">
+        <v>378</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="B189" s="4" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="4" t="s">
+        <v>842</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" s="4" t="s">
+        <v>843</v>
+      </c>
+      <c r="B191" s="4" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" s="4" t="s">
+        <v>844</v>
+      </c>
+      <c r="B192" s="4" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B193" s="4" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="5" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B194" s="5" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="4" t="s">
+        <v>846</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="4" t="s">
+        <v>847</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="4" t="s">
+        <v>848</v>
+      </c>
+      <c r="B197" s="4" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="B198" s="4" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="5" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B199" s="5" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="4" t="s">
+        <v>850</v>
+      </c>
+      <c r="B200" s="4" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="4" t="s">
+        <v>851</v>
+      </c>
+      <c r="B201" s="4" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="4" t="s">
+        <v>852</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="5" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B204" s="5" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="B206" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="B207" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B208" s="4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="B209" s="4" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="B210" s="4" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="B211" s="4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="B213" s="4" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B214" s="4" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B215" s="4" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="B216" s="4" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="B217" s="4" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B218" s="4" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="B219" s="4" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B220" s="4" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="B221" s="4" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="B222" s="4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B223" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="B225" s="4" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B226" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" s="4" t="s">
+        <v>428</v>
+      </c>
+      <c r="B227" s="4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="B228" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="B230" s="4" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="B231" s="4" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="B232" s="4" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="B233" s="4" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="B234" s="4" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="B235" s="4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="B236" s="4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="B237" s="4" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B238" s="4" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="B240" s="4" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="B241" s="4" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="B242" s="4" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="B243" s="4" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B244" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="B245" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B246" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="B247" s="4" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="B248" s="4" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="B249" s="4" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B250" s="4" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B251" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="B252" s="4" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B253" s="4" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="B254" s="4" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B255" s="4" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B256" s="4" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="B257" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A258" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="B258" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A259" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="B259" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A260" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="B260" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="B261" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="B262" s="4" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A263" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="B263" s="4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A264" s="4" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B264" s="4" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265" s="4" t="s">
+        <v>1175</v>
+      </c>
+      <c r="B265" s="4" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266" s="4" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B266" s="4" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A267" s="4" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B267" s="4" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A268" s="4" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B268" s="4" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A269" s="4" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B269" s="4" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A270" s="4" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B270" s="4" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271" s="4" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B271" s="4" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A272" s="4" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B272" s="4" t="s">
+        <v>1196</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A273" s="4" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B273" s="4" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274" s="4" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B274" s="4" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A275" s="4" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B275" s="4" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276" s="4" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B276" s="4" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277" s="4" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B277" s="4" t="s">
+        <v>1201</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278" s="4" t="s">
+        <v>1202</v>
+      </c>
+      <c r="B278" s="4" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279" s="4" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B279" s="4" t="s">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280" s="4" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B280" s="4" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281" s="4" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B281" s="4" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282" s="4" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B282" s="4" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A283" s="4" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B283" s="4" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284" s="4" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B284" s="4" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A285" s="4" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B285" s="4" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A286" s="4" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B286" s="4" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A287" s="4" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B287" s="4" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A288" s="4" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B288" s="4" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A289" s="4" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B289" s="4" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A290" s="4" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B290" s="4" t="s">
+        <v>1294</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A291" s="4" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B291" s="4" t="s">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A292" s="4" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B292" s="4" t="s">
+        <v>1298</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A293" s="4" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B293" s="4" t="s">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A294" s="4" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B294" s="4" t="s">
+        <v>1302</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A295" s="4" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B295" s="4" t="s">
+        <v>1304</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A296" s="4" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B296" s="4" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A297" s="4" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B297" s="4" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A298" t="s">
+        <v>191</v>
+      </c>
+      <c r="B298" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>198</v>
+      </c>
+      <c r="B299" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A300" t="s">
+        <v>207</v>
+      </c>
+      <c r="B300" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A301" t="s">
+        <v>192</v>
+      </c>
+      <c r="B301" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A302" t="s">
+        <v>199</v>
+      </c>
+      <c r="B302" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A303" t="s">
+        <v>208</v>
+      </c>
+      <c r="B303" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A304" t="s">
+        <v>193</v>
+      </c>
+      <c r="B304" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A305" t="s">
+        <v>200</v>
+      </c>
+      <c r="B305" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A306" t="s">
+        <v>209</v>
+      </c>
+      <c r="B306" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A651A7-E2A8-48DC-A289-3ADEDF80FEC9}">
   <dimension ref="A1:B309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A288" workbookViewId="0">
-      <selection activeCell="A310" sqref="A310"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18355,7 +20924,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6379954C-B519-4E67-8DE4-32A1851A1CD0}">
   <dimension ref="A1:D73"/>
   <sheetViews>
@@ -19405,7 +21974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB4B1FA-6628-4BA2-9F29-B27CBB154F46}">
   <dimension ref="A1:A120"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update cnt_inside to be numeric
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvisc1\Documents\projects\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32ECC0BF-58C9-4254-99D7-FCA691EDE36F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C9B960-627A-4F0F-A68F-7BC73D7B4035}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="6" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -16038,8 +16038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01158CBA-7E67-C246-925F-8A45600A7C89}">
   <dimension ref="A1:B306"/>
   <sheetViews>
-    <sheetView topLeftCell="A278" workbookViewId="0">
-      <selection activeCell="A298" sqref="A298:XFD298"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="A176" sqref="A176:B178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -18503,7 +18503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A651A7-E2A8-48DC-A289-3ADEDF80FEC9}">
   <dimension ref="A1:B312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
+    <sheetView topLeftCell="A110" workbookViewId="0">
       <selection activeCell="A143" sqref="A143"/>
     </sheetView>
   </sheetViews>
@@ -19604,7 +19604,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="142" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A142" s="5" t="s">
         <v>387</v>
       </c>
@@ -19636,7 +19636,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="146" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A146" s="5" t="s">
         <v>1238</v>
       </c>
@@ -19644,7 +19644,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="147" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A147" s="5" t="s">
         <v>391</v>
       </c>
@@ -19652,7 +19652,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="148" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A148" s="5" t="s">
         <v>392</v>
       </c>
@@ -19660,7 +19660,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="149" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A149" s="5" t="s">
         <v>393</v>
       </c>
@@ -19668,7 +19668,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="150" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A150" s="5" t="s">
         <v>394</v>
       </c>
@@ -19676,7 +19676,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="151" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A151" s="5" t="s">
         <v>395</v>
       </c>
@@ -19684,7 +19684,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="152" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A152" s="5" t="s">
         <v>396</v>
       </c>
@@ -19692,7 +19692,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="153" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A153" s="5" t="s">
         <v>397</v>
       </c>
@@ -19700,7 +19700,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="154" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A154" s="5" t="s">
         <v>398</v>
       </c>
@@ -19708,7 +19708,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="155" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A155" s="5" t="s">
         <v>399</v>
       </c>
@@ -19716,7 +19716,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="156" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A156" s="5" t="s">
         <v>400</v>
       </c>
@@ -19724,7 +19724,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="157" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A157" s="5" t="s">
         <v>401</v>
       </c>
@@ -19732,7 +19732,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="158" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A158" s="5" t="s">
         <v>1242</v>
       </c>
@@ -19740,7 +19740,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="159" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A159" s="5" t="s">
         <v>1243</v>
       </c>
@@ -19748,7 +19748,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="160" spans="1:2" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A160" s="5" t="s">
         <v>1244</v>
       </c>

</xml_diff>

<commit_message>
vaccination data and norway data
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/codebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8219B52-FDE8-D444-8A37-7769BB2C15C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64134DA9-6B5E-FA4E-94A1-8434F2F42DEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="28800" windowHeight="16640" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16260" activeTab="6" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="survey_3" sheetId="8" r:id="rId4"/>
     <sheet name="locations" sheetId="5" r:id="rId5"/>
     <sheet name="remove_vars" sheetId="6" r:id="rId6"/>
+    <sheet name="survey_norway" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">survey_1!$A$1:$G$423</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2659" uniqueCount="1239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3455" uniqueCount="1248">
   <si>
     <t>be01edu_me</t>
   </si>
@@ -3760,6 +3761,33 @@
   </si>
   <si>
     <t xml:space="preserve">locations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">educat_no </t>
+  </si>
+  <si>
+    <t>part_education_no</t>
+  </si>
+  <si>
+    <t>qno86</t>
+  </si>
+  <si>
+    <t>norway_green_spaces_comfort_86</t>
+  </si>
+  <si>
+    <t>qn082</t>
+  </si>
+  <si>
+    <t>qn083</t>
+  </si>
+  <si>
+    <t>qn084</t>
+  </si>
+  <si>
+    <t>qn085</t>
+  </si>
+  <si>
+    <t>no_region1</t>
   </si>
 </sst>
 </file>
@@ -4193,8 +4221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1C5985-D720-4533-B6F5-A2816F80F2F5}">
   <dimension ref="A1:B418"/>
   <sheetViews>
-    <sheetView topLeftCell="A403" workbookViewId="0">
-      <selection activeCell="B421" sqref="B421"/>
+    <sheetView topLeftCell="A400" workbookViewId="0">
+      <selection activeCell="B418" sqref="A1:B418"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14264,7 +14292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB4B1FA-6628-4BA2-9F29-B27CBB154F46}">
   <dimension ref="A1:A120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H208" sqref="H208"/>
     </sheetView>
   </sheetViews>
@@ -14879,4 +14907,3203 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FCB4066-218E-8F4E-956F-A6615E43F03A}">
+  <dimension ref="A1:B398"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A375" workbookViewId="0">
+      <selection activeCell="G393" sqref="G393"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>867</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>934</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>919</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>922</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>924</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>927</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>928</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>930</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>913</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>914</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>915</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
+        <v>868</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A137" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A138" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A139" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A140" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A147" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A148" s="2" t="s">
+        <v>870</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A150" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A151" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A152" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A154" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A155" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A156" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A157" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A158" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A159" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A160" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A165" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A166" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A167" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A168" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A169" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A170" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A171" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A172" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A173" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A174" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A175" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A176" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A202" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A203" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A204" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A205" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A206" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A207" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A208" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A212" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A213" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A214" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="2" t="s">
+        <v>873</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" s="2" t="s">
+        <v>874</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="2" t="s">
+        <v>876</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" s="2" t="s">
+        <v>877</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="2" t="s">
+        <v>878</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" s="2" t="s">
+        <v>881</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" s="2" t="s">
+        <v>886</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" s="2" t="s">
+        <v>882</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A229" s="2" t="s">
+        <v>884</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A230" s="2" t="s">
+        <v>885</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A231" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A232" s="2" t="s">
+        <v>888</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A233" s="2" t="s">
+        <v>889</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A234" s="2" t="s">
+        <v>890</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A235" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" s="2" t="s">
+        <v>893</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" s="2" t="s">
+        <v>895</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242" s="2" t="s">
+        <v>898</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243" s="2" t="s">
+        <v>899</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245" s="2" t="s">
+        <v>901</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247" s="2" t="s">
+        <v>903</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A258" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B258" s="2" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A259" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B259" s="2" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A260" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B260" s="2" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B261" s="2" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B262" s="2" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A263" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B263" s="2" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A264" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A267" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B267" s="2" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A268" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B268" s="2" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A269" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B269" s="2" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A270" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A272" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B272" s="2" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A273" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B273" s="2" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B274" s="2" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A275" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B275" s="2" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B276" s="2" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B277" s="2" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B278" s="2" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B279" s="2" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="B280" s="2" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="B281" s="2" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282" s="2" t="s">
+        <v>907</v>
+      </c>
+      <c r="B282" s="2" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A283" s="2" t="s">
+        <v>908</v>
+      </c>
+      <c r="B283" s="2" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="B284" s="2" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A285" s="2" t="s">
+        <v>910</v>
+      </c>
+      <c r="B285" s="2" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A286" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="B286" s="2" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A287" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="B287" s="2" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A288" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A289" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B289" s="2" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A290" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B290" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A291" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B291" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A292" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B292" s="2" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A293" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B293" s="2" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A294" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A295" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B295" s="2" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A296" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="B296" s="2" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A297" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B297" s="2" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A298" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A299" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B299" s="2" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A300" s="2" t="s">
+        <v>880</v>
+      </c>
+      <c r="B300" s="2" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A301" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A302" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A303" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A304" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="B304" s="2" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A305" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B305" s="2" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A306" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B306" s="2" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A307" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="B307" s="2" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A308" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A309" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A310" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="B310" s="2" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A311" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B311" s="2" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A312" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A313" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B313" s="2" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A314" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="B314" s="2" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A315" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B315" s="2" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A316" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B316" s="2" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A317" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B317" s="2" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A318" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B318" s="2" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A319" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="B319" s="2" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A320" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A321" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="B321" s="2" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A322" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="B322" s="2" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A323" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="B323" s="2" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A324" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="B324" s="2" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A325" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="B325" s="2" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A326" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A327" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A328" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="B328" s="2" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A329" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A330" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A331" s="2" t="s">
+        <v>785</v>
+      </c>
+      <c r="B331" s="2" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A332" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A333" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="B333" s="2" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A334" s="2" t="s">
+        <v>791</v>
+      </c>
+      <c r="B334" s="2" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A335" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="B335" s="2" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A336" s="2" t="s">
+        <v>795</v>
+      </c>
+      <c r="B336" s="2" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A337" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="B337" s="2" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A338" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="B338" s="2" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A339" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B339" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A340" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B340" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A341" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B341" s="2" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A342" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B342" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A343" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B343" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A344" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B344" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A345" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B345" s="2" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A346" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B346" s="2" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A347" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B347" s="2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A348" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B348" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A349" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B349" s="2" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A350" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B350" s="2" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A351" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="B351" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A352" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="B352" s="2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A353" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B353" s="2" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A354" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B354" s="2" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A355" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="B355" s="2" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A356" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="B356" s="2" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A357" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="B357" s="2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A358" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B358" s="2" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A359" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="B359" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A360" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="B360" s="2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A361" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="B361" s="2" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A362" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="B362" s="2" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A363" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="B363" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A364" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="B364" s="2" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A365" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B365" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A366" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B366" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A367" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B367" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A368" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B368" s="2" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A369" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B369" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A370" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B370" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A371" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B371" s="2" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A372" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B372" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A373" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B373" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A374" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="B374" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A375" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B375" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A376" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="B376" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A377" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="B377" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A378" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="B378" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A379" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="B379" s="2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A380" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B380" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A381" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B381" s="2" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A382" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="B382" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A383" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B383" s="2" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A384" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B384" s="2" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A385" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B385" s="2" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A386" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B386" s="2" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A387" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B387" s="2" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A388" s="2" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B388" s="2" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A389" s="2" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B389" s="2" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A390" s="2" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B390" s="2" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A391" s="2" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B391" s="2" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A392" s="2" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B392" s="2" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A393" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B393" s="2" t="s">
+        <v>1242</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A394" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B394" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A395" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B395" s="2" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A396" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B396" s="2" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A397" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B397" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A398" s="2" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B398" s="2" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
small updates to cleaning and spss_uk.xlsx
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amygimma/lshtm/comix_data_clean/codebook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8219B52-FDE8-D444-8A37-7769BB2C15C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE2F68F-35B7-654A-A186-98C0FBBBE9A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="580" windowWidth="28800" windowHeight="16640" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2659" uniqueCount="1239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2659" uniqueCount="1240">
   <si>
     <t>be01edu_me</t>
   </si>
@@ -3760,6 +3760,9 @@
   </si>
   <si>
     <t xml:space="preserve">locations </t>
+  </si>
+  <si>
+    <t>norway_physically_active_81</t>
   </si>
 </sst>
 </file>
@@ -4193,8 +4196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1C5985-D720-4533-B6F5-A2816F80F2F5}">
   <dimension ref="A1:B418"/>
   <sheetViews>
-    <sheetView topLeftCell="A403" workbookViewId="0">
-      <selection activeCell="B421" sqref="B421"/>
+    <sheetView tabSelected="1" topLeftCell="A372" workbookViewId="0">
+      <selection activeCell="B393" sqref="B393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7344,7 +7347,7 @@
         <v>202</v>
       </c>
       <c r="B393" t="s">
-        <v>936</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.2">
@@ -14264,8 +14267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB4B1FA-6628-4BA2-9F29-B27CBB154F46}">
   <dimension ref="A1:A120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H208" sqref="H208"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update remove var list
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wkerr\Dropbox\lshtm\CoMix\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9759DE4-A269-46D3-974A-4E46360AC813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744A880F-2427-4365-A5CE-761A1A94C9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="1273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2701" uniqueCount="1273">
   <si>
     <t>be01edu_me</t>
   </si>
@@ -14400,10 +14400,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB4B1FA-6628-4BA2-9F29-B27CBB154F46}">
-  <dimension ref="A1:A161"/>
+  <dimension ref="A1:A162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="A137" sqref="A137"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15216,6 +15216,11 @@
         <v>1272</v>
       </c>
     </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="4" t="s">
+        <v>224</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A481">
     <sortCondition ref="A2:A481"/>

</xml_diff>

<commit_message>
split remove vars excel sheet
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wkerr\Dropbox\lshtm\CoMix\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744A880F-2427-4365-A5CE-761A1A94C9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5515A00-294D-4583-AA60-334E772905FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="survey_3" sheetId="8" r:id="rId4"/>
     <sheet name="locations" sheetId="5" r:id="rId5"/>
     <sheet name="remove_vars" sheetId="6" r:id="rId6"/>
+    <sheet name="remove_vars_contact" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">survey_1!$A$1:$G$423</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2701" uniqueCount="1273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2821" uniqueCount="1273">
   <si>
     <t>be01edu_me</t>
   </si>
@@ -14402,7 +14403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB4B1FA-6628-4BA2-9F29-B27CBB154F46}">
   <dimension ref="A1:A162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+    <sheetView topLeftCell="A145" workbookViewId="0">
       <selection activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
@@ -15228,4 +15229,617 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C138C1C-F754-4981-8CD4-54939C29C320}">
+  <dimension ref="A1:A120"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
remove 0 in var_name
</commit_message>
<xml_diff>
--- a/codebook/var_names.xlsx
+++ b/codebook/var_names.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wkerr\Dropbox\lshtm\CoMix\comix_data_clean\codebook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DFC3D6-DA2F-465E-9122-39C13D17C918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10CF24B-BB81-4C7F-BDED-16696BB3603A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10410" yWindow="2610" windowWidth="21915" windowHeight="12720" firstSheet="1" activeTab="5" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{E3FB9B8D-729C-4B7A-BC06-409AAA905465}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="survey_3" sheetId="8" r:id="rId4"/>
     <sheet name="locations" sheetId="5" r:id="rId5"/>
     <sheet name="remove_vars" sheetId="6" r:id="rId6"/>
+    <sheet name="remove_vars_contact" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">survey_1!$A$1:$G$423</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2700" uniqueCount="1274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2821" uniqueCount="1274">
   <si>
     <t>be01edu_me</t>
   </si>
@@ -11057,8 +11058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2811056-AE3B-4304-B94A-E79692ED9D00}">
   <dimension ref="A1:B284"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11166,9 +11167,6 @@
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>236</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -14393,10 +14391,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAB4B1FA-6628-4BA2-9F29-B27CBB154F46}">
-  <dimension ref="A1:A161"/>
+  <dimension ref="A1:A162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A162" sqref="A162"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15209,10 +15207,633 @@
         <v>1273</v>
       </c>
     </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A481">
     <sortCondition ref="A2:A481"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8252FADE-D025-407D-A2A6-384F46289F4B}">
+  <dimension ref="A1:A120"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1081</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>1085</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>